<commit_message>
filter only term frequency
</commit_message>
<xml_diff>
--- a/FOMC1_bse.xlsx
+++ b/FOMC1_bse.xlsx
@@ -426,25 +426,25 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.0004584306812678286</v>
+        <v>0.006598627813926427</v>
       </c>
       <c r="C2">
-        <v>0.0007453611384166696</v>
+        <v>0.003877996505535535</v>
       </c>
       <c r="D2">
-        <v>3.601799477657799e-06</v>
+        <v>5.3937134934465e-05</v>
       </c>
       <c r="E2">
-        <v>0.0003606115335966238</v>
+        <v>0.003488863352990481</v>
       </c>
       <c r="F2">
-        <v>0.0001588352674506466</v>
+        <v>0.001528304686323664</v>
       </c>
       <c r="G2">
-        <v>6.496152950080003e-07</v>
+        <v>2.778739160693653e-06</v>
       </c>
       <c r="H2">
-        <v>0.001878767630491592</v>
+        <v>0.01640802561092625</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -452,25 +452,25 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.0004602316620969922</v>
+        <v>0.009322946936949543</v>
       </c>
       <c r="C3">
-        <v>0.0005830335558639192</v>
+        <v>0.0064001101109265</v>
       </c>
       <c r="D3">
-        <v>5.903307972425549e-06</v>
+        <v>7.320165137843136e-05</v>
       </c>
       <c r="E3">
-        <v>0.0002977364463293697</v>
+        <v>0.003834196372029334</v>
       </c>
       <c r="F3">
-        <v>0.0001512398829429841</v>
+        <v>0.001628218739132079</v>
       </c>
       <c r="G3">
-        <v>6.110484385546463e-07</v>
+        <v>2.693303077122159e-06</v>
       </c>
       <c r="H3">
-        <v>0.001539167920767613</v>
+        <v>0.01842455521026725</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -478,25 +478,25 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.0004977728111447627</v>
+        <v>0.007118264972926673</v>
       </c>
       <c r="C4">
-        <v>0.0008391827703404089</v>
+        <v>0.004833934953371188</v>
       </c>
       <c r="D4">
-        <v>7.743644753054611e-06</v>
+        <v>6.36157036938391e-05</v>
       </c>
       <c r="E4">
-        <v>0.0004039226527836899</v>
+        <v>0.00313088998046874</v>
       </c>
       <c r="F4">
-        <v>0.0001120288449629615</v>
+        <v>0.001638923475819724</v>
       </c>
       <c r="G4">
-        <v>4.780222854971025e-07</v>
+        <v>2.615147760572868e-06</v>
       </c>
       <c r="H4">
-        <v>0.00114332042402652</v>
+        <v>0.0185237414752938</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -504,25 +504,25 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.0004649358281501784</v>
+        <v>0.008067201392567594</v>
       </c>
       <c r="C5">
-        <v>0.0007031183897779323</v>
+        <v>0.005490822151255367</v>
       </c>
       <c r="D5">
-        <v>5.874883319832971e-06</v>
+        <v>8.429933491990937e-05</v>
       </c>
       <c r="E5">
-        <v>0.0003651121491717866</v>
+        <v>0.005504041496025222</v>
       </c>
       <c r="F5">
-        <v>0.0002222025231742086</v>
+        <v>0.0015857661754113</v>
       </c>
       <c r="G5">
-        <v>4.594940907489856e-07</v>
+        <v>2.187196333947552e-06</v>
       </c>
       <c r="H5">
-        <v>0.002348374710788982</v>
+        <v>0.01828987477585718</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -530,25 +530,25 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.0004490796340165827</v>
+        <v>0.007268740733079709</v>
       </c>
       <c r="C6">
-        <v>0.000448988353638087</v>
+        <v>0.006137553156708933</v>
       </c>
       <c r="D6">
-        <v>5.245709268451435e-06</v>
+        <v>6.885226550463696e-05</v>
       </c>
       <c r="E6">
-        <v>0.0003620338648280242</v>
+        <v>0.003612469396858488</v>
       </c>
       <c r="F6">
-        <v>0.0001445120257231271</v>
+        <v>0.0016935739569408</v>
       </c>
       <c r="G6">
-        <v>5.394090801900241e-07</v>
+        <v>2.375693541833269e-06</v>
       </c>
       <c r="H6">
-        <v>0.001557792560881087</v>
+        <v>0.01971596025899606</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -556,25 +556,25 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.0004658393073929673</v>
+        <v>0.006405945819602593</v>
       </c>
       <c r="C7">
-        <v>0.000593052116961216</v>
+        <v>0.004868857706434322</v>
       </c>
       <c r="D7">
-        <v>4.448997427676146e-06</v>
+        <v>6.139632916144347e-05</v>
       </c>
       <c r="E7">
-        <v>0.0003705323774591257</v>
+        <v>0.003345979704697023</v>
       </c>
       <c r="F7">
-        <v>0.0001889271277151352</v>
+        <v>0.001507350362748218</v>
       </c>
       <c r="G7">
-        <v>6.167350655576593e-07</v>
+        <v>2.335666688401791e-06</v>
       </c>
       <c r="H7">
-        <v>0.002164841094048366</v>
+        <v>0.01682081169456934</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -582,25 +582,25 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0.0003854379154984629</v>
+        <v>0.005676321930069526</v>
       </c>
       <c r="C8">
-        <v>0.0004387162921115578</v>
+        <v>0.005095019285593527</v>
       </c>
       <c r="D8">
-        <v>4.096567926928772e-06</v>
+        <v>6.564894424723373e-05</v>
       </c>
       <c r="E8">
-        <v>0.0003067583812969471</v>
+        <v>0.003567106907113196</v>
       </c>
       <c r="F8">
-        <v>0.0001254176245218871</v>
+        <v>0.001540176153685937</v>
       </c>
       <c r="G8">
-        <v>5.189044119074758e-07</v>
+        <v>2.568694907189377e-06</v>
       </c>
       <c r="H8">
-        <v>0.001612144325928802</v>
+        <v>0.01542986634920187</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -608,25 +608,25 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0.0003973041304425301</v>
+        <v>0.007041127685673809</v>
       </c>
       <c r="C9">
-        <v>0.0004043638278069232</v>
+        <v>0.004738669863752</v>
       </c>
       <c r="D9">
-        <v>4.409947405240877e-06</v>
+        <v>7.170329372164451e-05</v>
       </c>
       <c r="E9">
-        <v>0.000403714580234347</v>
+        <v>0.003726967327292638</v>
       </c>
       <c r="F9">
-        <v>0.0001264640861465681</v>
+        <v>0.001459897930673346</v>
       </c>
       <c r="G9">
-        <v>6.26526840885529e-07</v>
+        <v>2.405508714764885e-06</v>
       </c>
       <c r="H9">
-        <v>0.001531141003098299</v>
+        <v>0.01609926934311282</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -634,25 +634,25 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>0.0004363575582341993</v>
+        <v>0.007002811941816108</v>
       </c>
       <c r="C10">
-        <v>0.0004620916402119894</v>
+        <v>0.006413484274480179</v>
       </c>
       <c r="D10">
-        <v>5.276572982114781e-06</v>
+        <v>6.094482358405428e-05</v>
       </c>
       <c r="E10">
-        <v>0.0003444025347927136</v>
+        <v>0.004000304376732639</v>
       </c>
       <c r="F10">
-        <v>0.0001619084988991117</v>
+        <v>0.001534656057541524</v>
       </c>
       <c r="G10">
-        <v>5.04945663772531e-07</v>
+        <v>2.653872931646739e-06</v>
       </c>
       <c r="H10">
-        <v>0.001981976155696533</v>
+        <v>0.01763087386206696</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -660,25 +660,25 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>0.000520622542587606</v>
+        <v>0.005944964944837702</v>
       </c>
       <c r="C11">
-        <v>0.0004189226537688858</v>
+        <v>0.004409401921073281</v>
       </c>
       <c r="D11">
-        <v>5.034611021053066e-06</v>
+        <v>7.322084487517435e-05</v>
       </c>
       <c r="E11">
-        <v>0.0003948334007599052</v>
+        <v>0.003166407309783084</v>
       </c>
       <c r="F11">
-        <v>0.00019489997941229</v>
+        <v>0.001467353203421037</v>
       </c>
       <c r="G11">
-        <v>8.978000468546844e-07</v>
+        <v>2.288808021620401e-06</v>
       </c>
       <c r="H11">
-        <v>0.002059357310304782</v>
+        <v>0.01523376664369352</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -686,25 +686,25 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>0.0004311779018706855</v>
+        <v>0.006678066226250736</v>
       </c>
       <c r="C12">
-        <v>0.000543713020289437</v>
+        <v>0.005248952536851651</v>
       </c>
       <c r="D12">
-        <v>5.496574587601893e-06</v>
+        <v>6.596991345612327e-05</v>
       </c>
       <c r="E12">
-        <v>0.000314029275702369</v>
+        <v>0.003426838541486912</v>
       </c>
       <c r="F12">
-        <v>0.0001753312261797778</v>
+        <v>0.001577298018177348</v>
       </c>
       <c r="G12">
-        <v>5.734814102645085e-07</v>
+        <v>2.567951754046156e-06</v>
       </c>
       <c r="H12">
-        <v>0.001842319986576628</v>
+        <v>0.01725709066540041</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -712,25 +712,25 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>0.0005675213625996992</v>
+        <v>0.006775015288467712</v>
       </c>
       <c r="C13">
-        <v>0.0003425609639099354</v>
+        <v>0.008222632455479328</v>
       </c>
       <c r="D13">
-        <v>4.207456404522276e-06</v>
+        <v>7.381795773692006e-05</v>
       </c>
       <c r="E13">
-        <v>0.000384124034714634</v>
+        <v>0.004300991044882534</v>
       </c>
       <c r="F13">
-        <v>0.0001618876931795362</v>
+        <v>0.001857329470015968</v>
       </c>
       <c r="G13">
-        <v>4.566341773409485e-07</v>
+        <v>3.072015402968732e-06</v>
       </c>
       <c r="H13">
-        <v>0.001768759284215335</v>
+        <v>0.02006696128080938</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -738,25 +738,25 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>0.0004253470235233859</v>
+        <v>0.00644658417225049</v>
       </c>
       <c r="C14">
-        <v>0.0004260758095636375</v>
+        <v>0.005847106838582116</v>
       </c>
       <c r="D14">
-        <v>5.50769365829119e-06</v>
+        <v>5.352383116044223e-05</v>
       </c>
       <c r="E14">
-        <v>0.0004200649127487343</v>
+        <v>0.003868849070934175</v>
       </c>
       <c r="F14">
-        <v>0.0001382000118800635</v>
+        <v>0.001625864198028569</v>
       </c>
       <c r="G14">
-        <v>6.013254753175884e-07</v>
+        <v>2.231084378632263e-06</v>
       </c>
       <c r="H14">
-        <v>0.001627887061655732</v>
+        <v>0.01874621468934483</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -764,25 +764,25 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>0.0004744233035406893</v>
+        <v>0.006919738643903232</v>
       </c>
       <c r="C15">
-        <v>0.0004315314381983089</v>
+        <v>0.005505635039152803</v>
       </c>
       <c r="D15">
-        <v>5.442965415664332e-06</v>
+        <v>6.117773927555264e-05</v>
       </c>
       <c r="E15">
-        <v>0.0003373318332645573</v>
+        <v>0.00324353604640957</v>
       </c>
       <c r="F15">
-        <v>0.0001616644894506785</v>
+        <v>0.001452286229856082</v>
       </c>
       <c r="G15">
-        <v>6.18304749720929e-07</v>
+        <v>1.943132622413498e-06</v>
       </c>
       <c r="H15">
-        <v>0.001667814148627263</v>
+        <v>0.01873867351390217</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -790,25 +790,25 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>0.0005822399528460855</v>
+        <v>0.00808864117696147</v>
       </c>
       <c r="C16">
-        <v>0.0006837794088664846</v>
+        <v>0.00528038304456941</v>
       </c>
       <c r="D16">
-        <v>5.002702538216806e-06</v>
+        <v>6.196115025966717e-05</v>
       </c>
       <c r="E16">
-        <v>0.0004001004421990944</v>
+        <v>0.003708849528272289</v>
       </c>
       <c r="F16">
-        <v>0.0002552424533020736</v>
+        <v>0.001657070976254443</v>
       </c>
       <c r="G16">
-        <v>1.068989161899359e-06</v>
+        <v>2.602060537911755e-06</v>
       </c>
       <c r="H16">
-        <v>0.002647969479401599</v>
+        <v>0.01974113738935731</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -816,25 +816,25 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>0.0004249516064416896</v>
+        <v>0.005808086559523877</v>
       </c>
       <c r="C17">
-        <v>0.0005716365302429634</v>
+        <v>0.004680743689230209</v>
       </c>
       <c r="D17">
-        <v>4.889666923419936e-06</v>
+        <v>6.334574049718505e-05</v>
       </c>
       <c r="E17">
-        <v>0.0002684281293874045</v>
+        <v>0.003112701045037173</v>
       </c>
       <c r="F17">
-        <v>0.000127424064335088</v>
+        <v>0.001471920575907538</v>
       </c>
       <c r="G17">
-        <v>3.97977442901795e-07</v>
+        <v>2.174969525636597e-06</v>
       </c>
       <c r="H17">
-        <v>0.00136927590260386</v>
+        <v>0.01614787191559844</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -842,25 +842,25 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>0.0003919871858797127</v>
+        <v>0.006742636317651514</v>
       </c>
       <c r="C18">
-        <v>0.001166683622805948</v>
+        <v>0.005266327428079542</v>
       </c>
       <c r="D18">
-        <v>5.200215831309953e-06</v>
+        <v>6.255903856415757e-05</v>
       </c>
       <c r="E18">
-        <v>0.0004278328343057571</v>
+        <v>0.003808964428268076</v>
       </c>
       <c r="F18">
-        <v>0.0001789606193301155</v>
+        <v>0.001494759262056104</v>
       </c>
       <c r="G18">
-        <v>5.646756477080072e-07</v>
+        <v>2.564563655526817e-06</v>
       </c>
       <c r="H18">
-        <v>0.001932754647558373</v>
+        <v>0.01579615409164995</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -868,25 +868,25 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>0.0004998194960634594</v>
+        <v>0.006601091672568453</v>
       </c>
       <c r="C19">
-        <v>0.0007628256454668736</v>
+        <v>0.004460913419710401</v>
       </c>
       <c r="D19">
-        <v>5.596511436713497e-06</v>
+        <v>6.259988170460507e-05</v>
       </c>
       <c r="E19">
-        <v>0.000353807687460722</v>
+        <v>0.003468423867020155</v>
       </c>
       <c r="F19">
-        <v>0.0001436496920649401</v>
+        <v>0.001653287429040827</v>
       </c>
       <c r="G19">
-        <v>5.253884278380065e-07</v>
+        <v>2.468775067061119e-06</v>
       </c>
       <c r="H19">
-        <v>0.001641805555300029</v>
+        <v>0.01849205935439131</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -894,25 +894,25 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>0.000439073422988207</v>
+        <v>0.006220774505646781</v>
       </c>
       <c r="C20">
-        <v>0.0005501714763502382</v>
+        <v>0.01275226743732971</v>
       </c>
       <c r="D20">
-        <v>4.352086691670335e-06</v>
+        <v>7.087878595235893e-05</v>
       </c>
       <c r="E20">
-        <v>0.0004146421710223583</v>
+        <v>0.004879350317430295</v>
       </c>
       <c r="F20">
-        <v>0.0001299031650605685</v>
+        <v>0.001637169235907554</v>
       </c>
       <c r="G20">
-        <v>6.39987149254477e-07</v>
+        <v>2.368008175714512e-06</v>
       </c>
       <c r="H20">
-        <v>0.001337279781078984</v>
+        <v>0.01719002698760183</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -920,25 +920,25 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>0.0004250009288484349</v>
+        <v>0.007626022807700364</v>
       </c>
       <c r="C21">
-        <v>0.00039372528211927</v>
+        <v>0.006250600695640186</v>
       </c>
       <c r="D21">
-        <v>5.299266558972027e-06</v>
+        <v>6.305415519730159e-05</v>
       </c>
       <c r="E21">
-        <v>0.0003714973052376755</v>
+        <v>0.003392922114493343</v>
       </c>
       <c r="F21">
-        <v>0.0001514802882880033</v>
+        <v>0.001733501339015731</v>
       </c>
       <c r="G21">
-        <v>5.24329996178752e-07</v>
+        <v>2.241158634802071e-06</v>
       </c>
       <c r="H21">
-        <v>0.001775365523162549</v>
+        <v>0.01977971108889265</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -946,25 +946,25 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>0.0004697098963472451</v>
+        <v>0.006855513548270586</v>
       </c>
       <c r="C22">
-        <v>0.0005970688674357538</v>
+        <v>0.004505012518409662</v>
       </c>
       <c r="D22">
-        <v>4.768290507818101e-06</v>
+        <v>6.023076413242985e-05</v>
       </c>
       <c r="E22">
-        <v>0.0003361591843402609</v>
+        <v>0.003883009827904575</v>
       </c>
       <c r="F22">
-        <v>0.0001502244765892164</v>
+        <v>0.001736355562945185</v>
       </c>
       <c r="G22">
-        <v>5.714505233589665e-07</v>
+        <v>3.137325450389668e-06</v>
       </c>
       <c r="H22">
-        <v>0.001625561381566282</v>
+        <v>0.01829711484515944</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -972,25 +972,25 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>0.0003704603835412333</v>
+        <v>0.007097864325018914</v>
       </c>
       <c r="C23">
-        <v>0.0004520997815466961</v>
+        <v>0.004412343979989111</v>
       </c>
       <c r="D23">
-        <v>3.958144379207295e-06</v>
+        <v>7.52153431021791e-05</v>
       </c>
       <c r="E23">
-        <v>0.0003699954835974817</v>
+        <v>0.003706632994364059</v>
       </c>
       <c r="F23">
-        <v>0.0001460183277981508</v>
+        <v>0.001584041416265937</v>
       </c>
       <c r="G23">
-        <v>4.652649523661742e-07</v>
+        <v>2.695647686893602e-06</v>
       </c>
       <c r="H23">
-        <v>0.0016762905345485</v>
+        <v>0.01646269645685316</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -998,25 +998,25 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>0.0004891704076033734</v>
+        <v>0.008708220934678677</v>
       </c>
       <c r="C24">
-        <v>0.0003552987912105793</v>
+        <v>0.005923651001529981</v>
       </c>
       <c r="D24">
-        <v>4.124048835501096e-06</v>
+        <v>6.326031313580606e-05</v>
       </c>
       <c r="E24">
-        <v>0.0002987737313183167</v>
+        <v>0.004613413378012723</v>
       </c>
       <c r="F24">
-        <v>0.0001555065997894831</v>
+        <v>0.001586688026078141</v>
       </c>
       <c r="G24">
-        <v>6.412315599274924e-07</v>
+        <v>2.7871544065083e-06</v>
       </c>
       <c r="H24">
-        <v>0.001689055527283375</v>
+        <v>0.01808884575166774</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1024,25 +1024,25 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>0.0004140389188963074</v>
+        <v>0.006396037957056814</v>
       </c>
       <c r="C25">
-        <v>0.0003306420596464281</v>
+        <v>0.00518810848331116</v>
       </c>
       <c r="D25">
-        <v>4.662047837200564e-06</v>
+        <v>6.429017750365504e-05</v>
       </c>
       <c r="E25">
-        <v>0.0002951336536012815</v>
+        <v>0.003254465789853041</v>
       </c>
       <c r="F25">
-        <v>0.0001119642134873412</v>
+        <v>0.001418538995544199</v>
       </c>
       <c r="G25">
-        <v>4.827315937165553e-07</v>
+        <v>2.346368426859994e-06</v>
       </c>
       <c r="H25">
-        <v>0.001269242280526751</v>
+        <v>0.01579155299092889</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1050,25 +1050,25 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>0.0005001794082115365</v>
+        <v>0.007076236445484481</v>
       </c>
       <c r="C26">
-        <v>0.0005764203235045327</v>
+        <v>0.005048219384468389</v>
       </c>
       <c r="D26">
-        <v>4.517832894921769e-06</v>
+        <v>6.08029187650978e-05</v>
       </c>
       <c r="E26">
-        <v>0.0003537007355264587</v>
+        <v>0.00313397108440972</v>
       </c>
       <c r="F26">
-        <v>0.0001592640888508069</v>
+        <v>0.001593192822055468</v>
       </c>
       <c r="G26">
-        <v>5.738326572710582e-07</v>
+        <v>2.468824404562564e-06</v>
       </c>
       <c r="H26">
-        <v>0.001714355412751286</v>
+        <v>0.01772593651920305</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -1076,25 +1076,25 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>0.0004602419260638791</v>
+        <v>0.007470903768964923</v>
       </c>
       <c r="C27">
-        <v>0.0005883703852740322</v>
+        <v>0.005339207664550817</v>
       </c>
       <c r="D27">
-        <v>3.879238566540062e-06</v>
+        <v>5.729701828656795e-05</v>
       </c>
       <c r="E27">
-        <v>0.000292822399976626</v>
+        <v>0.003723743436859817</v>
       </c>
       <c r="F27">
-        <v>0.0001222006982904115</v>
+        <v>0.001642558834134377</v>
       </c>
       <c r="G27">
-        <v>5.042740835719952e-07</v>
+        <v>2.831450426772739e-06</v>
       </c>
       <c r="H27">
-        <v>0.001500052335310131</v>
+        <v>0.01863717756802747</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -1102,25 +1102,25 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>0.0005178192138800496</v>
+        <v>0.007739067380536753</v>
       </c>
       <c r="C28">
-        <v>0.0006152939610744316</v>
+        <v>0.004869582699993435</v>
       </c>
       <c r="D28">
-        <v>4.902967165256604e-06</v>
+        <v>6.61439298458809e-05</v>
       </c>
       <c r="E28">
-        <v>0.0003293557973404883</v>
+        <v>0.003703016405711951</v>
       </c>
       <c r="F28">
-        <v>0.0001654859371223645</v>
+        <v>0.001691654464380077</v>
       </c>
       <c r="G28">
-        <v>4.371499115056406e-07</v>
+        <v>2.745418266229265e-06</v>
       </c>
       <c r="H28">
-        <v>0.001963458436884294</v>
+        <v>0.01852858808642712</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -1128,25 +1128,25 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>0.000375519989893701</v>
+        <v>0.006211261118673294</v>
       </c>
       <c r="C29">
-        <v>0.0004271016605090632</v>
+        <v>0.004787757918540174</v>
       </c>
       <c r="D29">
-        <v>5.34865496465458e-06</v>
+        <v>5.718121692949249e-05</v>
       </c>
       <c r="E29">
-        <v>0.0003203302340827016</v>
+        <v>0.003046429781311208</v>
       </c>
       <c r="F29">
-        <v>0.0001916971656565408</v>
+        <v>0.001542589117534346</v>
       </c>
       <c r="G29">
-        <v>4.191563962620785e-07</v>
+        <v>2.462497928556546e-06</v>
       </c>
       <c r="H29">
-        <v>0.002201204010857001</v>
+        <v>0.01708897709414916</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1154,25 +1154,25 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>0.0004521779471181519</v>
+        <v>0.006245361766451894</v>
       </c>
       <c r="C30">
-        <v>0.0007990543274336715</v>
+        <v>0.005559178717289947</v>
       </c>
       <c r="D30">
-        <v>5.290235144228539e-06</v>
+        <v>7.195949518982706e-05</v>
       </c>
       <c r="E30">
-        <v>0.0003156449169118358</v>
+        <v>0.003670918708845829</v>
       </c>
       <c r="F30">
-        <v>0.0001584527379804501</v>
+        <v>0.001406217424182136</v>
       </c>
       <c r="G30">
-        <v>4.417527623839792e-07</v>
+        <v>2.299596251512571e-06</v>
       </c>
       <c r="H30">
-        <v>0.001795524544212995</v>
+        <v>0.01514456477171922</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1180,25 +1180,25 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>0.0004468692233816904</v>
+        <v>0.007613866753241585</v>
       </c>
       <c r="C31">
-        <v>0.000492905234663112</v>
+        <v>0.007360486630758568</v>
       </c>
       <c r="D31">
-        <v>5.679578749690389e-06</v>
+        <v>6.164450673186877e-05</v>
       </c>
       <c r="E31">
-        <v>0.0003842281249073933</v>
+        <v>0.003938600767602681</v>
       </c>
       <c r="F31">
-        <v>0.0001569795080825558</v>
+        <v>0.001777874068396953</v>
       </c>
       <c r="G31">
-        <v>4.40539444902438e-07</v>
+        <v>2.657649676694689e-06</v>
       </c>
       <c r="H31">
-        <v>0.001911545008133366</v>
+        <v>0.02028627391076841</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1206,25 +1206,25 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>0.000474704529246345</v>
+        <v>0.007083147021626596</v>
       </c>
       <c r="C32">
-        <v>0.0005875505908807365</v>
+        <v>0.005411822491201511</v>
       </c>
       <c r="D32">
-        <v>6.568405351953423e-06</v>
+        <v>6.753413922331581e-05</v>
       </c>
       <c r="E32">
-        <v>0.0004195008005605518</v>
+        <v>0.003973791596140541</v>
       </c>
       <c r="F32">
-        <v>0.0001450384471217292</v>
+        <v>0.001534596838805665</v>
       </c>
       <c r="G32">
-        <v>6.181924094038865e-07</v>
+        <v>2.387488014156639e-06</v>
       </c>
       <c r="H32">
-        <v>0.001689227331341955</v>
+        <v>0.01604991779327344</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -1232,25 +1232,25 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>0.0005191409798589239</v>
+        <v>0.00606241382383437</v>
       </c>
       <c r="C33">
-        <v>0.000767819485356283</v>
+        <v>0.007432257854941613</v>
       </c>
       <c r="D33">
-        <v>5.424761835060324e-06</v>
+        <v>5.834685616320966e-05</v>
       </c>
       <c r="E33">
-        <v>0.0003193120759958462</v>
+        <v>0.003609747342699688</v>
       </c>
       <c r="F33">
-        <v>0.0001307019088875994</v>
+        <v>0.001625397089490505</v>
       </c>
       <c r="G33">
-        <v>5.340942937000828e-07</v>
+        <v>2.659911015651508e-06</v>
       </c>
       <c r="H33">
-        <v>0.001444945030908068</v>
+        <v>0.01655008901635933</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -1258,25 +1258,25 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>0.0005369398566328012</v>
+        <v>0.005568902242959925</v>
       </c>
       <c r="C34">
-        <v>0.0003504091316888854</v>
+        <v>0.004693770959790787</v>
       </c>
       <c r="D34">
-        <v>4.657286013296314e-06</v>
+        <v>6.403820710319948e-05</v>
       </c>
       <c r="E34">
-        <v>0.000344508753055067</v>
+        <v>0.0031751863134045</v>
       </c>
       <c r="F34">
-        <v>0.0001560739824870935</v>
+        <v>0.001360074390761674</v>
       </c>
       <c r="G34">
-        <v>5.075204582431318e-07</v>
+        <v>2.037197644768211e-06</v>
       </c>
       <c r="H34">
-        <v>0.001918218687048842</v>
+        <v>0.01492403121958798</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -1284,25 +1284,25 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>0.0003612684995887925</v>
+        <v>0.007357740247345924</v>
       </c>
       <c r="C35">
-        <v>0.0003118348330261772</v>
+        <v>0.004317690951115822</v>
       </c>
       <c r="D35">
-        <v>4.043495298713494e-06</v>
+        <v>6.744246657963925e-05</v>
       </c>
       <c r="E35">
-        <v>0.0003692018320697151</v>
+        <v>0.003481553496400743</v>
       </c>
       <c r="F35">
-        <v>0.0001385339664440797</v>
+        <v>0.001644254684328278</v>
       </c>
       <c r="G35">
-        <v>4.807960340455846e-07</v>
+        <v>2.50023408857236e-06</v>
       </c>
       <c r="H35">
-        <v>0.001461668728984082</v>
+        <v>0.01825724071150686</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -1310,25 +1310,25 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>0.0005181790494510126</v>
+        <v>0.006478888344574412</v>
       </c>
       <c r="C36">
-        <v>0.0005214310393953815</v>
+        <v>0.006285098889358124</v>
       </c>
       <c r="D36">
-        <v>5.324659330697047e-06</v>
+        <v>5.819825879948397e-05</v>
       </c>
       <c r="E36">
-        <v>0.0004225717180609767</v>
+        <v>0.004425637103943542</v>
       </c>
       <c r="F36">
-        <v>0.0002369043858482699</v>
+        <v>0.001713952106916065</v>
       </c>
       <c r="G36">
-        <v>8.730556468091281e-07</v>
+        <v>2.862105474102389e-06</v>
       </c>
       <c r="H36">
-        <v>0.002350757793576126</v>
+        <v>0.01854763631530637</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -1336,25 +1336,25 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>0.0004625638267196526</v>
+        <v>0.005799247096555602</v>
       </c>
       <c r="C37">
-        <v>0.0004522943746551606</v>
+        <v>0.004315052029110756</v>
       </c>
       <c r="D37">
-        <v>4.745040157531817e-06</v>
+        <v>4.810279337219539e-05</v>
       </c>
       <c r="E37">
-        <v>0.000377690585909264</v>
+        <v>0.003072571991131067</v>
       </c>
       <c r="F37">
-        <v>0.0001343113437802216</v>
+        <v>0.001853000267322652</v>
       </c>
       <c r="G37">
-        <v>5.833307253058235e-07</v>
+        <v>3.105211023951264e-06</v>
       </c>
       <c r="H37">
-        <v>0.001662849823836866</v>
+        <v>0.01965200223795589</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -1362,25 +1362,25 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>0.0004488339962394349</v>
+        <v>0.006557480665729385</v>
       </c>
       <c r="C38">
-        <v>0.0006263573947758093</v>
+        <v>0.005966497962696628</v>
       </c>
       <c r="D38">
-        <v>5.980756566018636e-06</v>
+        <v>5.224563052108204e-05</v>
       </c>
       <c r="E38">
-        <v>0.0003946172422385671</v>
+        <v>0.003392886270336638</v>
       </c>
       <c r="F38">
-        <v>0.0001588542930644675</v>
+        <v>0.001569145966327028</v>
       </c>
       <c r="G38">
-        <v>5.852219502217648e-07</v>
+        <v>2.543069000877411e-06</v>
       </c>
       <c r="H38">
-        <v>0.001629214012294277</v>
+        <v>0.01730224354861146</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -1388,25 +1388,25 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>0.0003486815965853534</v>
+        <v>0.007999068383857531</v>
       </c>
       <c r="C39">
-        <v>0.0005653174352591669</v>
+        <v>0.004895368220164689</v>
       </c>
       <c r="D39">
-        <v>4.423440923860507e-06</v>
+        <v>7.96440851890627e-05</v>
       </c>
       <c r="E39">
-        <v>0.0003745290835367757</v>
+        <v>0.003920655434825706</v>
       </c>
       <c r="F39">
-        <v>0.0001414550627864193</v>
+        <v>0.001629178603406511</v>
       </c>
       <c r="G39">
-        <v>5.580959768592082e-07</v>
+        <v>2.583361774776979e-06</v>
       </c>
       <c r="H39">
-        <v>0.00149479102326523</v>
+        <v>0.0190721239069263</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -1414,25 +1414,25 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>0.0005571061386552312</v>
+        <v>0.005257846167422173</v>
       </c>
       <c r="C40">
-        <v>0.0005579757400255908</v>
+        <v>0.006168855468188292</v>
       </c>
       <c r="D40">
-        <v>6.128780481461964e-06</v>
+        <v>5.993423877464775e-05</v>
       </c>
       <c r="E40">
-        <v>0.0003748013821465801</v>
+        <v>0.002990139925416239</v>
       </c>
       <c r="F40">
-        <v>0.0001866143980126336</v>
+        <v>0.001307233168486027</v>
       </c>
       <c r="G40">
-        <v>5.475423363565161e-07</v>
+        <v>2.31001704144121e-06</v>
       </c>
       <c r="H40">
-        <v>0.00221688292310874</v>
+        <v>0.0140372442188852</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -1440,25 +1440,25 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>0.0005642252079848455</v>
+        <v>0.008584276914987407</v>
       </c>
       <c r="C41">
-        <v>0.0005422667788888369</v>
+        <v>0.005682950909476501</v>
       </c>
       <c r="D41">
-        <v>6.509559518137327e-06</v>
+        <v>6.787760813098265e-05</v>
       </c>
       <c r="E41">
-        <v>0.0003703563907826945</v>
+        <v>0.004450274999483269</v>
       </c>
       <c r="F41">
-        <v>0.00017127750311433</v>
+        <v>0.00158939135662838</v>
       </c>
       <c r="G41">
-        <v>5.037778099396796e-07</v>
+        <v>2.506396640176041e-06</v>
       </c>
       <c r="H41">
-        <v>0.001867579438424068</v>
+        <v>0.01868240425032123</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -1466,25 +1466,25 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>0.0004900198003944056</v>
+        <v>0.007207016830690294</v>
       </c>
       <c r="C42">
-        <v>0.0007593054584784277</v>
+        <v>0.005705317242084512</v>
       </c>
       <c r="D42">
-        <v>5.772481467315494e-06</v>
+        <v>5.860523370707246e-05</v>
       </c>
       <c r="E42">
-        <v>0.0003321329251131711</v>
+        <v>0.004362253777742681</v>
       </c>
       <c r="F42">
-        <v>0.0001571297011687908</v>
+        <v>0.001729998176711146</v>
       </c>
       <c r="G42">
-        <v>6.341844357434474e-07</v>
+        <v>2.791729020461972e-06</v>
       </c>
       <c r="H42">
-        <v>0.001623933650364747</v>
+        <v>0.01864551834445006</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -1492,25 +1492,25 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>0.000414311726400956</v>
+        <v>0.006487922519527556</v>
       </c>
       <c r="C43">
-        <v>0.0005274217487966556</v>
+        <v>0.005130880477689261</v>
       </c>
       <c r="D43">
-        <v>5.575705696395991e-06</v>
+        <v>5.981102347500397e-05</v>
       </c>
       <c r="E43">
-        <v>0.000417996780622622</v>
+        <v>0.003278347003345101</v>
       </c>
       <c r="F43">
-        <v>0.0001518929401364857</v>
+        <v>0.001534876408474067</v>
       </c>
       <c r="G43">
-        <v>5.511375366576239e-07</v>
+        <v>2.602487126078917e-06</v>
       </c>
       <c r="H43">
-        <v>0.001712980666499665</v>
+        <v>0.01640807661299193</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -1518,25 +1518,25 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>0.000470312422846236</v>
+        <v>0.007271771623906549</v>
       </c>
       <c r="C44">
-        <v>0.0005723655447193948</v>
+        <v>0.004505504683204373</v>
       </c>
       <c r="D44">
-        <v>4.783069713446366e-06</v>
+        <v>6.662842835946537e-05</v>
       </c>
       <c r="E44">
-        <v>0.0003897385389797696</v>
+        <v>0.003871627354301604</v>
       </c>
       <c r="F44">
-        <v>0.0001523944718394436</v>
+        <v>0.001570538678010946</v>
       </c>
       <c r="G44">
-        <v>5.9560585870496e-07</v>
+        <v>2.289966302724293e-06</v>
       </c>
       <c r="H44">
-        <v>0.001624788951144415</v>
+        <v>0.01721402799656972</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -1544,25 +1544,25 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>0.0003865931705414426</v>
+        <v>0.006190569144013266</v>
       </c>
       <c r="C45">
-        <v>0.0009622280325967637</v>
+        <v>0.007608132133116384</v>
       </c>
       <c r="D45">
-        <v>5.413562735821325e-06</v>
+        <v>8.313064829364811e-05</v>
       </c>
       <c r="E45">
-        <v>0.0003246703340854221</v>
+        <v>0.004020179876304788</v>
       </c>
       <c r="F45">
-        <v>0.0001278646069294889</v>
+        <v>0.001435675916717356</v>
       </c>
       <c r="G45">
-        <v>5.052899545468172e-07</v>
+        <v>2.421449948928657e-06</v>
       </c>
       <c r="H45">
-        <v>0.001440999094480535</v>
+        <v>0.01516078813066327</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -1570,25 +1570,25 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <v>0.0003151365011038439</v>
+        <v>0.007101178262841693</v>
       </c>
       <c r="C46">
-        <v>0.000446939321581393</v>
+        <v>0.004385382172069081</v>
       </c>
       <c r="D46">
-        <v>3.814050401771491e-06</v>
+        <v>6.675688215876106e-05</v>
       </c>
       <c r="E46">
-        <v>0.0003033734575003205</v>
+        <v>0.003129012624322459</v>
       </c>
       <c r="F46">
-        <v>0.000115324998391746</v>
+        <v>0.001755489974478339</v>
       </c>
       <c r="G46">
-        <v>3.804425116677524e-07</v>
+        <v>3.015256322208439e-06</v>
       </c>
       <c r="H46">
-        <v>0.001419974167902045</v>
+        <v>0.01958098172024488</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -1596,25 +1596,25 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>0.0004922714466249136</v>
+        <v>0.007065036622471754</v>
       </c>
       <c r="C47">
-        <v>0.0008406978565870377</v>
+        <v>0.005571761619958947</v>
       </c>
       <c r="D47">
-        <v>4.64410988248556e-06</v>
+        <v>7.000407125951572e-05</v>
       </c>
       <c r="E47">
-        <v>0.0003683517869282058</v>
+        <v>0.003886447865985293</v>
       </c>
       <c r="F47">
-        <v>0.0001510378886292248</v>
+        <v>0.00156922930617613</v>
       </c>
       <c r="G47">
-        <v>5.320459269185994e-07</v>
+        <v>2.599659733101384e-06</v>
       </c>
       <c r="H47">
-        <v>0.001520469114246474</v>
+        <v>0.01692763733180697</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -1622,25 +1622,25 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>0.0004407752282857974</v>
+        <v>0.007514065055150852</v>
       </c>
       <c r="C48">
-        <v>0.0008092184925381224</v>
+        <v>0.00475962608425535</v>
       </c>
       <c r="D48">
-        <v>6.324983528503404e-06</v>
+        <v>6.942048987237778e-05</v>
       </c>
       <c r="E48">
-        <v>0.0003466822902240312</v>
+        <v>0.004084583657486452</v>
       </c>
       <c r="F48">
-        <v>0.0001759159823422957</v>
+        <v>0.001591580891100075</v>
       </c>
       <c r="G48">
-        <v>5.829198002621618e-07</v>
+        <v>2.481992980860043e-06</v>
       </c>
       <c r="H48">
-        <v>0.00205894703812772</v>
+        <v>0.01808337342984878</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -1648,25 +1648,25 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>0.0005563223267239933</v>
+        <v>0.01218559991834068</v>
       </c>
       <c r="C49">
-        <v>0.000445550418514187</v>
+        <v>0.005329879517643832</v>
       </c>
       <c r="D49">
-        <v>4.648523019459353e-06</v>
+        <v>6.728659995967473e-05</v>
       </c>
       <c r="E49">
-        <v>0.000329180754384593</v>
+        <v>0.004857976542506702</v>
       </c>
       <c r="F49">
-        <v>0.0001630053716079285</v>
+        <v>0.001935643454478484</v>
       </c>
       <c r="G49">
-        <v>4.507995795658893e-07</v>
+        <v>7.917762987811322e-06</v>
       </c>
       <c r="H49">
-        <v>0.001798111197770245</v>
+        <v>0.02107087581567014</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -1674,25 +1674,25 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>0.0004112874263548252</v>
+        <v>0.006630444531873675</v>
       </c>
       <c r="C50">
-        <v>0.000529771282958258</v>
+        <v>0.005162134812369424</v>
       </c>
       <c r="D50">
-        <v>5.246312420419503e-06</v>
+        <v>7.744258552936261e-05</v>
       </c>
       <c r="E50">
-        <v>0.0002901418258735436</v>
+        <v>0.003052237962733767</v>
       </c>
       <c r="F50">
-        <v>0.0001180733322128241</v>
+        <v>0.001602899526406107</v>
       </c>
       <c r="G50">
-        <v>4.61014256535732e-07</v>
+        <v>2.651770823935734e-06</v>
       </c>
       <c r="H50">
-        <v>0.001257872043583131</v>
+        <v>0.01811599305023153</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -1700,25 +1700,25 @@
         <v>49</v>
       </c>
       <c r="B51">
-        <v>0.0005025882202534775</v>
+        <v>0.006702975991447859</v>
       </c>
       <c r="C51">
-        <v>0.0005974243749937929</v>
+        <v>0.005426485484627935</v>
       </c>
       <c r="D51">
-        <v>4.569097286030428e-06</v>
+        <v>5.972650736894883e-05</v>
       </c>
       <c r="E51">
-        <v>0.0003288567079180718</v>
+        <v>0.003471524607473756</v>
       </c>
       <c r="F51">
-        <v>0.0001547640442932289</v>
+        <v>0.001818738946496014</v>
       </c>
       <c r="G51">
-        <v>4.789193031296676e-07</v>
+        <v>2.931771750136725e-06</v>
       </c>
       <c r="H51">
-        <v>0.001786170449301971</v>
+        <v>0.01990922519129997</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -1726,25 +1726,25 @@
         <v>50</v>
       </c>
       <c r="B52">
-        <v>0.0004311956013892845</v>
+        <v>0.007114195437340132</v>
       </c>
       <c r="C52">
-        <v>0.0009516186625469617</v>
+        <v>0.005216434957635158</v>
       </c>
       <c r="D52">
-        <v>5.043606539226971e-06</v>
+        <v>7.425855544716846e-05</v>
       </c>
       <c r="E52">
-        <v>0.0003313448762319931</v>
+        <v>0.003460342318850336</v>
       </c>
       <c r="F52">
-        <v>0.0001804098176631764</v>
+        <v>0.001803814185668604</v>
       </c>
       <c r="G52">
-        <v>5.76396619410141e-07</v>
+        <v>2.62714620499932e-06</v>
       </c>
       <c r="H52">
-        <v>0.002058681372253766</v>
+        <v>0.02086508670864159</v>
       </c>
     </row>
     <row r="53" spans="1:8">
@@ -1752,25 +1752,25 @@
         <v>51</v>
       </c>
       <c r="B53">
-        <v>0.0004527697054264578</v>
+        <v>0.007876673175107089</v>
       </c>
       <c r="C53">
-        <v>0.0007110956490566404</v>
+        <v>0.005045702774384455</v>
       </c>
       <c r="D53">
-        <v>5.543392003249345e-06</v>
+        <v>5.61975088764884e-05</v>
       </c>
       <c r="E53">
-        <v>0.0003538530425252114</v>
+        <v>0.004022667201729083</v>
       </c>
       <c r="F53">
-        <v>0.0001433198848836399</v>
+        <v>0.001842786072667841</v>
       </c>
       <c r="G53">
-        <v>6.025272964774901e-07</v>
+        <v>2.923192440511913e-06</v>
       </c>
       <c r="H53">
-        <v>0.001677731266086899</v>
+        <v>0.02109675800175666</v>
       </c>
     </row>
     <row r="54" spans="1:8">
@@ -1778,25 +1778,25 @@
         <v>52</v>
       </c>
       <c r="B54">
-        <v>0.0004629475223486102</v>
+        <v>0.005732424832246321</v>
       </c>
       <c r="C54">
-        <v>0.0004534964107215853</v>
+        <v>0.004487390015650886</v>
       </c>
       <c r="D54">
-        <v>4.666501049210186e-06</v>
+        <v>5.153025888013809e-05</v>
       </c>
       <c r="E54">
-        <v>0.0003903934408428911</v>
+        <v>0.003151152982276787</v>
       </c>
       <c r="F54">
-        <v>0.0001618130256039626</v>
+        <v>0.001271027838997191</v>
       </c>
       <c r="G54">
-        <v>6.134399714452574e-07</v>
+        <v>2.131963244745936e-06</v>
       </c>
       <c r="H54">
-        <v>0.001910923195397351</v>
+        <v>0.01533821333078384</v>
       </c>
     </row>
     <row r="55" spans="1:8">
@@ -1804,25 +1804,25 @@
         <v>53</v>
       </c>
       <c r="B55">
-        <v>0.0004335512691216046</v>
+        <v>0.006977225810534471</v>
       </c>
       <c r="C55">
-        <v>0.0005426855433500944</v>
+        <v>0.005209275935208764</v>
       </c>
       <c r="D55">
-        <v>4.222714009066062e-06</v>
+        <v>6.040145433239832e-05</v>
       </c>
       <c r="E55">
-        <v>0.0003761333472297486</v>
+        <v>0.003564898015403354</v>
       </c>
       <c r="F55">
-        <v>0.0001440820798551025</v>
+        <v>0.001786342758486153</v>
       </c>
       <c r="G55">
-        <v>4.714246604323561e-07</v>
+        <v>3.351495604778694e-06</v>
       </c>
       <c r="H55">
-        <v>0.001644958976274724</v>
+        <v>0.01835212777121649</v>
       </c>
     </row>
     <row r="56" spans="1:8">
@@ -1830,25 +1830,25 @@
         <v>54</v>
       </c>
       <c r="B56">
-        <v>0.0004961375482868354</v>
+        <v>0.006469681842026904</v>
       </c>
       <c r="C56">
-        <v>0.0004027816330424279</v>
+        <v>0.005866092581405087</v>
       </c>
       <c r="D56">
-        <v>5.052200392974099e-06</v>
+        <v>6.020336818613886e-05</v>
       </c>
       <c r="E56">
-        <v>0.0003547383011443329</v>
+        <v>0.003892970813676729</v>
       </c>
       <c r="F56">
-        <v>0.000149999414816942</v>
+        <v>0.001520355235774778</v>
       </c>
       <c r="G56">
-        <v>5.52518410786396e-07</v>
+        <v>2.056774199033118e-06</v>
       </c>
       <c r="H56">
-        <v>0.001683290966676619</v>
+        <v>0.01835684521779223</v>
       </c>
     </row>
     <row r="57" spans="1:8">
@@ -1856,25 +1856,25 @@
         <v>55</v>
       </c>
       <c r="B57">
-        <v>0.0005187487894656478</v>
+        <v>0.006828669038607928</v>
       </c>
       <c r="C57">
-        <v>0.0005900325775782074</v>
+        <v>0.004616796922447711</v>
       </c>
       <c r="D57">
-        <v>5.319507969340162e-06</v>
+        <v>6.595718067952607e-05</v>
       </c>
       <c r="E57">
-        <v>0.0004350331189920949</v>
+        <v>0.003649652161052749</v>
       </c>
       <c r="F57">
-        <v>0.0001870393968306044</v>
+        <v>0.001627844952127305</v>
       </c>
       <c r="G57">
-        <v>6.372655190630282e-07</v>
+        <v>2.658268885351173e-06</v>
       </c>
       <c r="H57">
-        <v>0.002170997971284931</v>
+        <v>0.01741522522384265</v>
       </c>
     </row>
     <row r="58" spans="1:8">
@@ -1882,25 +1882,25 @@
         <v>56</v>
       </c>
       <c r="B58">
-        <v>0.0004537598506558446</v>
+        <v>0.00553299659922534</v>
       </c>
       <c r="C58">
-        <v>0.0004853067643166996</v>
+        <v>0.005033766575786702</v>
       </c>
       <c r="D58">
-        <v>4.715024166447287e-06</v>
+        <v>5.934716570782109e-05</v>
       </c>
       <c r="E58">
-        <v>0.0004005949212221586</v>
+        <v>0.003288838213386725</v>
       </c>
       <c r="F58">
-        <v>0.0001453554852539791</v>
+        <v>0.001657015711474516</v>
       </c>
       <c r="G58">
-        <v>5.423450015237498e-07</v>
+        <v>2.737981251572082e-06</v>
       </c>
       <c r="H58">
-        <v>0.001736253521823225</v>
+        <v>0.01721446693654441</v>
       </c>
     </row>
     <row r="59" spans="1:8">
@@ -1908,25 +1908,25 @@
         <v>57</v>
       </c>
       <c r="B59">
-        <v>0.0003592677207195472</v>
+        <v>0.007484752130217654</v>
       </c>
       <c r="C59">
-        <v>0.0005420586056614111</v>
+        <v>0.00532029096086683</v>
       </c>
       <c r="D59">
-        <v>5.1654513182791e-06</v>
+        <v>5.348856504757189e-05</v>
       </c>
       <c r="E59">
-        <v>0.0002626279813345465</v>
+        <v>0.004487190384391675</v>
       </c>
       <c r="F59">
-        <v>0.0001717834149168552</v>
+        <v>0.001904126362549884</v>
       </c>
       <c r="G59">
-        <v>4.468144338997783e-07</v>
+        <v>2.807275936957789e-06</v>
       </c>
       <c r="H59">
-        <v>0.001806722841830688</v>
+        <v>0.02250507844636165</v>
       </c>
     </row>
     <row r="60" spans="1:8">
@@ -1934,25 +1934,25 @@
         <v>58</v>
       </c>
       <c r="B60">
-        <v>0.0005790314442754456</v>
+        <v>0.007597158422131753</v>
       </c>
       <c r="C60">
-        <v>0.0004790737520294587</v>
+        <v>0.00484745081991078</v>
       </c>
       <c r="D60">
-        <v>6.095609067150521e-06</v>
+        <v>6.199464619353022e-05</v>
       </c>
       <c r="E60">
-        <v>0.0004458117676648919</v>
+        <v>0.003372401575851719</v>
       </c>
       <c r="F60">
-        <v>0.0002164859946069558</v>
+        <v>0.001607165425685789</v>
       </c>
       <c r="G60">
-        <v>6.550867677386577e-07</v>
+        <v>2.720098381661838e-06</v>
       </c>
       <c r="H60">
-        <v>0.002380369746835342</v>
+        <v>0.01781188616349567</v>
       </c>
     </row>
     <row r="61" spans="1:8">
@@ -1960,25 +1960,25 @@
         <v>59</v>
       </c>
       <c r="B61">
-        <v>0.0005059534860299315</v>
+        <v>0.00649231020017476</v>
       </c>
       <c r="C61">
-        <v>0.0006134167323341543</v>
+        <v>0.004651309530595978</v>
       </c>
       <c r="D61">
-        <v>5.880918613125991e-06</v>
+        <v>5.93935625779794e-05</v>
       </c>
       <c r="E61">
-        <v>0.0004181111241885128</v>
+        <v>0.003371742691065188</v>
       </c>
       <c r="F61">
-        <v>0.0001838892182600686</v>
+        <v>0.001415441181486409</v>
       </c>
       <c r="G61">
-        <v>6.530251627135531e-07</v>
+        <v>2.379605229297126e-06</v>
       </c>
       <c r="H61">
-        <v>0.001991532611497652</v>
+        <v>0.01624474872118348</v>
       </c>
     </row>
     <row r="62" spans="1:8">
@@ -1986,25 +1986,25 @@
         <v>60</v>
       </c>
       <c r="B62">
-        <v>0.0003392340435233688</v>
+        <v>0.007349724145290578</v>
       </c>
       <c r="C62">
-        <v>0.0006225504817992593</v>
+        <v>0.006068394366393488</v>
       </c>
       <c r="D62">
-        <v>4.410720888755566e-06</v>
+        <v>5.919530381430438e-05</v>
       </c>
       <c r="E62">
-        <v>0.0003304383881044868</v>
+        <v>0.002973432774156608</v>
       </c>
       <c r="F62">
-        <v>0.0001421157540060974</v>
+        <v>0.001564546527604893</v>
       </c>
       <c r="G62">
-        <v>4.364745931247189e-07</v>
+        <v>2.562182439821475e-06</v>
       </c>
       <c r="H62">
-        <v>0.001605804475078263</v>
+        <v>0.01833517924148642</v>
       </c>
     </row>
     <row r="63" spans="1:8">
@@ -2012,25 +2012,25 @@
         <v>61</v>
       </c>
       <c r="B63">
-        <v>0.000410688987963029</v>
+        <v>0.008058894195513068</v>
       </c>
       <c r="C63">
-        <v>0.0006005796673913955</v>
+        <v>0.005334288441004058</v>
       </c>
       <c r="D63">
-        <v>4.278489948893731e-06</v>
+        <v>5.53862068688723e-05</v>
       </c>
       <c r="E63">
-        <v>0.0003020023410820126</v>
+        <v>0.005215114183975084</v>
       </c>
       <c r="F63">
-        <v>0.0001321258547749564</v>
+        <v>0.001613166831678034</v>
       </c>
       <c r="G63">
-        <v>3.609886164163494e-07</v>
+        <v>2.870247819349435e-06</v>
       </c>
       <c r="H63">
-        <v>0.001524476614327534</v>
+        <v>0.02113011716368897</v>
       </c>
     </row>
     <row r="64" spans="1:8">
@@ -2038,25 +2038,25 @@
         <v>62</v>
       </c>
       <c r="B64">
-        <v>0.0003823285817732349</v>
+        <v>0.00671366467182723</v>
       </c>
       <c r="C64">
-        <v>0.0004221802992362773</v>
+        <v>0.006457652683942111</v>
       </c>
       <c r="D64">
-        <v>5.205466905039986e-06</v>
+        <v>8.153158215172906e-05</v>
       </c>
       <c r="E64">
-        <v>0.0003406016872937324</v>
+        <v>0.003503166554865961</v>
       </c>
       <c r="F64">
-        <v>0.0001524685307377124</v>
+        <v>0.001502389136358189</v>
       </c>
       <c r="G64">
-        <v>4.071906370349529e-07</v>
+        <v>2.42075830496031e-06</v>
       </c>
       <c r="H64">
-        <v>0.001920859328751427</v>
+        <v>0.01726609480787675</v>
       </c>
     </row>
     <row r="65" spans="1:8">
@@ -2064,25 +2064,25 @@
         <v>63</v>
       </c>
       <c r="B65">
-        <v>0.0004132706562343275</v>
+        <v>0.008397593651383557</v>
       </c>
       <c r="C65">
-        <v>0.0003644055452777253</v>
+        <v>0.004481088135365009</v>
       </c>
       <c r="D65">
-        <v>4.599712409623586e-06</v>
+        <v>6.142226442408274e-05</v>
       </c>
       <c r="E65">
-        <v>0.0003398103772082814</v>
+        <v>0.004658142651660455</v>
       </c>
       <c r="F65">
-        <v>0.0001542556188375237</v>
+        <v>0.001522412099900389</v>
       </c>
       <c r="G65">
-        <v>5.43596079191012e-07</v>
+        <v>2.689410425763483e-06</v>
       </c>
       <c r="H65">
-        <v>0.001649025048008388</v>
+        <v>0.01693762541472594</v>
       </c>
     </row>
     <row r="66" spans="1:8">
@@ -2090,25 +2090,25 @@
         <v>64</v>
       </c>
       <c r="B66">
-        <v>0.0003983162359252568</v>
+        <v>0.005705941237302352</v>
       </c>
       <c r="C66">
-        <v>0.001077222654581702</v>
+        <v>0.005436005706974067</v>
       </c>
       <c r="D66">
-        <v>4.312220806442227e-06</v>
+        <v>5.620841044192583e-05</v>
       </c>
       <c r="E66">
-        <v>0.0002843475558169713</v>
+        <v>0.003596717683160761</v>
       </c>
       <c r="F66">
-        <v>0.0001478668699173758</v>
+        <v>0.001338733542250932</v>
       </c>
       <c r="G66">
-        <v>5.345521453542941e-07</v>
+        <v>2.239439075835489e-06</v>
       </c>
       <c r="H66">
-        <v>0.001805666619524501</v>
+        <v>0.01377056384933092</v>
       </c>
     </row>
     <row r="67" spans="1:8">
@@ -2116,25 +2116,25 @@
         <v>65</v>
       </c>
       <c r="B67">
-        <v>0.0004047749307100086</v>
+        <v>0.00546387072098457</v>
       </c>
       <c r="C67">
-        <v>0.000373565454477449</v>
+        <v>0.009536947423093085</v>
       </c>
       <c r="D67">
-        <v>4.442310730071443e-06</v>
+        <v>4.428096812476228e-05</v>
       </c>
       <c r="E67">
-        <v>0.0003638257339828833</v>
+        <v>0.004433440149447988</v>
       </c>
       <c r="F67">
-        <v>0.0001664010988285233</v>
+        <v>0.001573486626035931</v>
       </c>
       <c r="G67">
-        <v>5.770701311422911e-07</v>
+        <v>2.244135464466614e-06</v>
       </c>
       <c r="H67">
-        <v>0.001860795722132298</v>
+        <v>0.01726249565038644</v>
       </c>
     </row>
     <row r="68" spans="1:8">
@@ -2142,25 +2142,25 @@
         <v>66</v>
       </c>
       <c r="B68">
-        <v>0.00048337802067038</v>
+        <v>0.006560960633642383</v>
       </c>
       <c r="C68">
-        <v>0.001201179151995602</v>
+        <v>0.004390638846107406</v>
       </c>
       <c r="D68">
-        <v>6.209287010653825e-06</v>
+        <v>4.617328014879823e-05</v>
       </c>
       <c r="E68">
-        <v>0.000287690276210421</v>
+        <v>0.004516178977149576</v>
       </c>
       <c r="F68">
-        <v>0.00016139756904995</v>
+        <v>0.001556475702636486</v>
       </c>
       <c r="G68">
-        <v>5.674484682809073e-07</v>
+        <v>2.33975782860266e-06</v>
       </c>
       <c r="H68">
-        <v>0.001906638382100041</v>
+        <v>0.01852080992325497</v>
       </c>
     </row>
     <row r="69" spans="1:8">
@@ -2168,25 +2168,25 @@
         <v>67</v>
       </c>
       <c r="B69">
-        <v>0.0005648399524920118</v>
+        <v>0.006760088678347128</v>
       </c>
       <c r="C69">
-        <v>0.0004614682915632635</v>
+        <v>0.004400875020385809</v>
       </c>
       <c r="D69">
-        <v>7.216396901876023e-06</v>
+        <v>7.172509068901521e-05</v>
       </c>
       <c r="E69">
-        <v>0.0004498412786561613</v>
+        <v>0.003569484733497529</v>
       </c>
       <c r="F69">
-        <v>0.0001552588891251939</v>
+        <v>0.00137895055971173</v>
       </c>
       <c r="G69">
-        <v>7.521681663069953e-07</v>
+        <v>2.416120793138529e-06</v>
       </c>
       <c r="H69">
-        <v>0.001906510009669119</v>
+        <v>0.0148596438315643</v>
       </c>
     </row>
     <row r="70" spans="1:8">
@@ -2194,25 +2194,25 @@
         <v>68</v>
       </c>
       <c r="B70">
-        <v>0.0004215380194121785</v>
+        <v>0.006820121996687282</v>
       </c>
       <c r="C70">
-        <v>0.0003206700074032188</v>
+        <v>0.005117055132813232</v>
       </c>
       <c r="D70">
-        <v>4.557449942737399e-06</v>
+        <v>5.614441075283114e-05</v>
       </c>
       <c r="E70">
-        <v>0.0003814495919710789</v>
+        <v>0.004016124768260411</v>
       </c>
       <c r="F70">
-        <v>0.0001410516528329544</v>
+        <v>0.001598577202628533</v>
       </c>
       <c r="G70">
-        <v>4.854418903576125e-07</v>
+        <v>2.63962613815915e-06</v>
       </c>
       <c r="H70">
-        <v>0.001637688324201392</v>
+        <v>0.01868912048333492</v>
       </c>
     </row>
     <row r="71" spans="1:8">
@@ -2220,25 +2220,25 @@
         <v>69</v>
       </c>
       <c r="B71">
-        <v>0.000504618985818842</v>
+        <v>0.006959061865676693</v>
       </c>
       <c r="C71">
-        <v>0.0005869430728006941</v>
+        <v>0.006181615603296687</v>
       </c>
       <c r="D71">
-        <v>4.289782137730155e-06</v>
+        <v>4.986137238217529e-05</v>
       </c>
       <c r="E71">
-        <v>0.0003487803678535391</v>
+        <v>0.003866448991851886</v>
       </c>
       <c r="F71">
-        <v>0.0001682558703308825</v>
+        <v>0.001680134498240864</v>
       </c>
       <c r="G71">
-        <v>5.440756580947746e-07</v>
+        <v>2.441914496462157e-06</v>
       </c>
       <c r="H71">
-        <v>0.002153377736047884</v>
+        <v>0.01927622607619412</v>
       </c>
     </row>
     <row r="72" spans="1:8">
@@ -2246,25 +2246,25 @@
         <v>70</v>
       </c>
       <c r="B72">
-        <v>0.0003985176245047274</v>
+        <v>0.00851882452447752</v>
       </c>
       <c r="C72">
-        <v>0.0007067288634314237</v>
+        <v>0.003963288819612358</v>
       </c>
       <c r="D72">
-        <v>4.731949004629965e-06</v>
+        <v>4.980880295940959e-05</v>
       </c>
       <c r="E72">
-        <v>0.0004168912378081471</v>
+        <v>0.004013033913195717</v>
       </c>
       <c r="F72">
-        <v>0.0001747215464368882</v>
+        <v>0.001670984694815799</v>
       </c>
       <c r="G72">
-        <v>6.320584226101889e-07</v>
+        <v>4.605696700114517e-06</v>
       </c>
       <c r="H72">
-        <v>0.00187191875296988</v>
+        <v>0.01844307029472019</v>
       </c>
     </row>
     <row r="73" spans="1:8">
@@ -2272,25 +2272,25 @@
         <v>71</v>
       </c>
       <c r="B73">
-        <v>0.0004682344766696002</v>
+        <v>0.00864392843236159</v>
       </c>
       <c r="C73">
-        <v>0.000661219281085754</v>
+        <v>0.006161874041629057</v>
       </c>
       <c r="D73">
-        <v>5.967763723746843e-06</v>
+        <v>6.879418163255648e-05</v>
       </c>
       <c r="E73">
-        <v>0.0004125675565611248</v>
+        <v>0.003857951013347994</v>
       </c>
       <c r="F73">
-        <v>0.0001662078744400796</v>
+        <v>0.001515249028203149</v>
       </c>
       <c r="G73">
-        <v>5.900258441785706e-07</v>
+        <v>3.026278580811796e-06</v>
       </c>
       <c r="H73">
-        <v>0.002040790175919861</v>
+        <v>0.01844592336603649</v>
       </c>
     </row>
     <row r="74" spans="1:8">
@@ -2298,25 +2298,25 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>0.0003535632355573551</v>
+        <v>0.007289776927994866</v>
       </c>
       <c r="C74">
-        <v>0.0005144249155998931</v>
+        <v>0.005722882060830731</v>
       </c>
       <c r="D74">
-        <v>5.519524510042117e-06</v>
+        <v>6.184724299201252e-05</v>
       </c>
       <c r="E74">
-        <v>0.0003830250834749488</v>
+        <v>0.003407916186144866</v>
       </c>
       <c r="F74">
-        <v>0.0001624610044705109</v>
+        <v>0.001812746167095278</v>
       </c>
       <c r="G74">
-        <v>4.805275068935391e-07</v>
+        <v>3.308239397216921e-06</v>
       </c>
       <c r="H74">
-        <v>0.001686118867281864</v>
+        <v>0.02023340870034883</v>
       </c>
     </row>
     <row r="75" spans="1:8">
@@ -2324,25 +2324,25 @@
         <v>73</v>
       </c>
       <c r="B75">
-        <v>0.0004145115626528958</v>
+        <v>0.006045755150590249</v>
       </c>
       <c r="C75">
-        <v>0.0007354487709334712</v>
+        <v>0.006886968467471897</v>
       </c>
       <c r="D75">
-        <v>4.477758101596686e-06</v>
+        <v>5.942011807729384e-05</v>
       </c>
       <c r="E75">
-        <v>0.0003291120738356063</v>
+        <v>0.003293143366265841</v>
       </c>
       <c r="F75">
-        <v>0.0001193038727185976</v>
+        <v>0.001539726043452342</v>
       </c>
       <c r="G75">
-        <v>5.138383555149127e-07</v>
+        <v>2.233627938774672e-06</v>
       </c>
       <c r="H75">
-        <v>0.001515093451444736</v>
+        <v>0.01736117506158497</v>
       </c>
     </row>
     <row r="76" spans="1:8">
@@ -2350,25 +2350,25 @@
         <v>74</v>
       </c>
       <c r="B76">
-        <v>0.000522996274008144</v>
+        <v>0.008493368442225344</v>
       </c>
       <c r="C76">
-        <v>0.0003954189049467287</v>
+        <v>0.005009895975447354</v>
       </c>
       <c r="D76">
-        <v>5.902989026994134e-06</v>
+        <v>7.6285548014428e-05</v>
       </c>
       <c r="E76">
-        <v>0.0003983969378798616</v>
+        <v>0.00338363773494996</v>
       </c>
       <c r="F76">
-        <v>0.0001607137872820795</v>
+        <v>0.002202050182032023</v>
       </c>
       <c r="G76">
-        <v>4.871113848313855e-07</v>
+        <v>3.481105332212004e-06</v>
       </c>
       <c r="H76">
-        <v>0.001822839868103411</v>
+        <v>0.02314229000857908</v>
       </c>
     </row>
     <row r="77" spans="1:8">
@@ -2376,25 +2376,25 @@
         <v>75</v>
       </c>
       <c r="B77">
-        <v>0.0004655552183976898</v>
+        <v>0.00675278524015299</v>
       </c>
       <c r="C77">
-        <v>0.0005645697051076333</v>
+        <v>0.004880000430847682</v>
       </c>
       <c r="D77">
-        <v>4.537327105678919e-06</v>
+        <v>5.098298525481482e-05</v>
       </c>
       <c r="E77">
-        <v>0.000326438639262647</v>
+        <v>0.003883252831622501</v>
       </c>
       <c r="F77">
-        <v>0.000147557049767955</v>
+        <v>0.0015527430650491</v>
       </c>
       <c r="G77">
-        <v>4.958126248855492e-07</v>
+        <v>3.085431375716479e-06</v>
       </c>
       <c r="H77">
-        <v>0.001860266473509962</v>
+        <v>0.01726751208662927</v>
       </c>
     </row>
     <row r="78" spans="1:8">
@@ -2402,25 +2402,25 @@
         <v>76</v>
       </c>
       <c r="B78">
-        <v>0.0004835333037424473</v>
+        <v>0.007833115308140126</v>
       </c>
       <c r="C78">
-        <v>0.0004067751790801319</v>
+        <v>0.006718457698258191</v>
       </c>
       <c r="D78">
-        <v>4.446517930656418e-06</v>
+        <v>6.036959991083842e-05</v>
       </c>
       <c r="E78">
-        <v>0.0004177757774368651</v>
+        <v>0.005206565554895065</v>
       </c>
       <c r="F78">
-        <v>0.0001584348142081795</v>
+        <v>0.001903372763951846</v>
       </c>
       <c r="G78">
-        <v>5.171498248726289e-07</v>
+        <v>3.297503093485144e-06</v>
       </c>
       <c r="H78">
-        <v>0.001779200072331589</v>
+        <v>0.0207238863754352</v>
       </c>
     </row>
     <row r="79" spans="1:8">
@@ -2428,25 +2428,25 @@
         <v>77</v>
       </c>
       <c r="B79">
-        <v>0.0003675332608985368</v>
+        <v>0.007199861136624922</v>
       </c>
       <c r="C79">
-        <v>0.0004329926214814441</v>
+        <v>0.004822828876214259</v>
       </c>
       <c r="D79">
-        <v>3.645172926307336e-06</v>
+        <v>7.19562706168627e-05</v>
       </c>
       <c r="E79">
-        <v>0.0003378579262262007</v>
+        <v>0.003501865106088513</v>
       </c>
       <c r="F79">
-        <v>0.0001576178725192983</v>
+        <v>0.001391098619195431</v>
       </c>
       <c r="G79">
-        <v>4.925658231321267e-07</v>
+        <v>2.019008484036473e-06</v>
       </c>
       <c r="H79">
-        <v>0.001649737383607264</v>
+        <v>0.01612334554450237</v>
       </c>
     </row>
     <row r="80" spans="1:8">
@@ -2454,25 +2454,25 @@
         <v>78</v>
       </c>
       <c r="B80">
-        <v>0.0005099663320466306</v>
+        <v>0.007055403835613634</v>
       </c>
       <c r="C80">
-        <v>0.0005261765552787246</v>
+        <v>0.006829215825083402</v>
       </c>
       <c r="D80">
-        <v>6.03082550774553e-06</v>
+        <v>5.858959354469513e-05</v>
       </c>
       <c r="E80">
-        <v>0.0003976910109739679</v>
+        <v>0.003247960309130435</v>
       </c>
       <c r="F80">
-        <v>0.0001701107828022341</v>
+        <v>0.002227359167129981</v>
       </c>
       <c r="G80">
-        <v>6.175368831937066e-07</v>
+        <v>3.451660698837649e-06</v>
       </c>
       <c r="H80">
-        <v>0.001965699239795855</v>
+        <v>0.02350443984438422</v>
       </c>
     </row>
     <row r="81" spans="1:8">
@@ -2480,25 +2480,25 @@
         <v>79</v>
       </c>
       <c r="B81">
-        <v>0.0004795630309177175</v>
+        <v>0.005820251326175244</v>
       </c>
       <c r="C81">
-        <v>0.0004834243805787268</v>
+        <v>0.00508020511641211</v>
       </c>
       <c r="D81">
-        <v>5.773046256378191e-06</v>
+        <v>6.778046838010356e-05</v>
       </c>
       <c r="E81">
-        <v>0.0004190136243429671</v>
+        <v>0.002968525035384588</v>
       </c>
       <c r="F81">
-        <v>0.0001783383836648882</v>
+        <v>0.001431765813326998</v>
       </c>
       <c r="G81">
-        <v>6.542800183356521e-07</v>
+        <v>2.384449766279267e-06</v>
       </c>
       <c r="H81">
-        <v>0.001828274291796568</v>
+        <v>0.01574065715971855</v>
       </c>
     </row>
     <row r="82" spans="1:8">
@@ -2506,25 +2506,25 @@
         <v>80</v>
       </c>
       <c r="B82">
-        <v>0.0004936464479491581</v>
+        <v>0.006572939371993888</v>
       </c>
       <c r="C82">
-        <v>0.0008858841433643328</v>
+        <v>0.00351123151166257</v>
       </c>
       <c r="D82">
-        <v>8.536391601383886e-06</v>
+        <v>5.972876604835036e-05</v>
       </c>
       <c r="E82">
-        <v>0.000423827347828764</v>
+        <v>0.003300239308623305</v>
       </c>
       <c r="F82">
-        <v>0.0001471696029652331</v>
+        <v>0.001519953561804344</v>
       </c>
       <c r="G82">
-        <v>4.222766207616204e-07</v>
+        <v>2.249482134181459e-06</v>
       </c>
       <c r="H82">
-        <v>0.001510093168315923</v>
+        <v>0.01659394968942894</v>
       </c>
     </row>
     <row r="83" spans="1:8">
@@ -2532,25 +2532,25 @@
         <v>81</v>
       </c>
       <c r="B83">
-        <v>0.000432753111570369</v>
+        <v>0.006451030621910344</v>
       </c>
       <c r="C83">
-        <v>0.0004262439415754814</v>
+        <v>0.007286994245829679</v>
       </c>
       <c r="D83">
-        <v>4.228670116455886e-06</v>
+        <v>7.217975614560694e-05</v>
       </c>
       <c r="E83">
-        <v>0.0003777228211600774</v>
+        <v>0.003863106489959392</v>
       </c>
       <c r="F83">
-        <v>0.0001566646087412327</v>
+        <v>0.001663481567538973</v>
       </c>
       <c r="G83">
-        <v>5.168739786940906e-07</v>
+        <v>2.78794532315264e-06</v>
       </c>
       <c r="H83">
-        <v>0.001948420943281012</v>
+        <v>0.0174750476381876</v>
       </c>
     </row>
     <row r="84" spans="1:8">
@@ -2558,25 +2558,25 @@
         <v>82</v>
       </c>
       <c r="B84">
-        <v>0.0005126701073776328</v>
+        <v>0.006527182544829108</v>
       </c>
       <c r="C84">
-        <v>0.000436770169012</v>
+        <v>0.004656851897466109</v>
       </c>
       <c r="D84">
-        <v>4.860531580207492e-06</v>
+        <v>7.77067376952912e-05</v>
       </c>
       <c r="E84">
-        <v>0.0003930744288803137</v>
+        <v>0.003779506593356589</v>
       </c>
       <c r="F84">
-        <v>0.0001774997676956815</v>
+        <v>0.001458337715358868</v>
       </c>
       <c r="G84">
-        <v>6.162017488988242e-07</v>
+        <v>2.378676931613301e-06</v>
       </c>
       <c r="H84">
-        <v>0.001934411838309737</v>
+        <v>0.01602731496734838</v>
       </c>
     </row>
     <row r="85" spans="1:8">
@@ -2584,25 +2584,25 @@
         <v>83</v>
       </c>
       <c r="B85">
-        <v>0.0004099615262736334</v>
+        <v>0.00592060063319322</v>
       </c>
       <c r="C85">
-        <v>0.0006957983127640155</v>
+        <v>0.004655642221472845</v>
       </c>
       <c r="D85">
-        <v>4.948858466014397e-06</v>
+        <v>5.347101907578758e-05</v>
       </c>
       <c r="E85">
-        <v>0.0003072323682036497</v>
+        <v>0.003187324739084202</v>
       </c>
       <c r="F85">
-        <v>0.000154688152576105</v>
+        <v>0.001465618517289672</v>
       </c>
       <c r="G85">
-        <v>6.712592865972715e-07</v>
+        <v>2.153595635057068e-06</v>
       </c>
       <c r="H85">
-        <v>0.001599759698245694</v>
+        <v>0.01585781047509004</v>
       </c>
     </row>
     <row r="86" spans="1:8">
@@ -2610,25 +2610,25 @@
         <v>84</v>
       </c>
       <c r="B86">
-        <v>0.000540304434918415</v>
+        <v>0.007191525541910728</v>
       </c>
       <c r="C86">
-        <v>0.0005037804028395945</v>
+        <v>0.005903187856504768</v>
       </c>
       <c r="D86">
-        <v>5.82011249824638e-06</v>
+        <v>6.080479369394197e-05</v>
       </c>
       <c r="E86">
-        <v>0.0004225889683875781</v>
+        <v>0.003881192326874905</v>
       </c>
       <c r="F86">
-        <v>0.0002113947857990242</v>
+        <v>0.001851538350348037</v>
       </c>
       <c r="G86">
-        <v>6.005305428570444e-07</v>
+        <v>3.280268771681201e-06</v>
       </c>
       <c r="H86">
-        <v>0.002206705844994786</v>
+        <v>0.01944415921966859</v>
       </c>
     </row>
     <row r="87" spans="1:8">
@@ -2636,25 +2636,25 @@
         <v>85</v>
       </c>
       <c r="B87">
-        <v>0.000337166541600519</v>
+        <v>0.006334452943650663</v>
       </c>
       <c r="C87">
-        <v>0.0007804330747624508</v>
+        <v>0.004140615967998197</v>
       </c>
       <c r="D87">
-        <v>5.327992929725748e-06</v>
+        <v>5.848021492276929e-05</v>
       </c>
       <c r="E87">
-        <v>0.0002990097993388775</v>
+        <v>0.00319628054051272</v>
       </c>
       <c r="F87">
-        <v>0.0001271234432020442</v>
+        <v>0.001326903428121143</v>
       </c>
       <c r="G87">
-        <v>4.574114337142561e-07</v>
+        <v>2.445718214389359e-06</v>
       </c>
       <c r="H87">
-        <v>0.001243158252973414</v>
+        <v>0.0153671926753339</v>
       </c>
     </row>
     <row r="88" spans="1:8">
@@ -2662,25 +2662,25 @@
         <v>86</v>
       </c>
       <c r="B88">
-        <v>0.0004471696216226012</v>
+        <v>0.005718448666035877</v>
       </c>
       <c r="C88">
-        <v>0.0004961701676105941</v>
+        <v>0.005494157381457357</v>
       </c>
       <c r="D88">
-        <v>5.188082385274702e-06</v>
+        <v>5.999340893919511e-05</v>
       </c>
       <c r="E88">
-        <v>0.0003645951796674823</v>
+        <v>0.00301781719403285</v>
       </c>
       <c r="F88">
-        <v>0.0001410701782341143</v>
+        <v>0.001464716306511431</v>
       </c>
       <c r="G88">
-        <v>5.679183092578717e-07</v>
+        <v>2.586039357558383e-06</v>
       </c>
       <c r="H88">
-        <v>0.001749029788761756</v>
+        <v>0.01590784673255196</v>
       </c>
     </row>
     <row r="89" spans="1:8">
@@ -2688,25 +2688,25 @@
         <v>87</v>
       </c>
       <c r="B89">
-        <v>0.0004762465861443757</v>
+        <v>0.006659452567668837</v>
       </c>
       <c r="C89">
-        <v>0.0005958422902280263</v>
+        <v>0.005822042565237187</v>
       </c>
       <c r="D89">
-        <v>5.913646096341375e-06</v>
+        <v>5.997233529889172e-05</v>
       </c>
       <c r="E89">
-        <v>0.0003543244990338931</v>
+        <v>0.003478653679108751</v>
       </c>
       <c r="F89">
-        <v>0.0001755894042062896</v>
+        <v>0.002174824646581518</v>
       </c>
       <c r="G89">
-        <v>5.655826020186044e-07</v>
+        <v>3.68339213615605e-06</v>
       </c>
       <c r="H89">
-        <v>0.002206068996857176</v>
+        <v>0.02121487478380614</v>
       </c>
     </row>
     <row r="90" spans="1:8">
@@ -2714,25 +2714,25 @@
         <v>88</v>
       </c>
       <c r="B90">
-        <v>0.0004310598314579808</v>
+        <v>0.007114025659220497</v>
       </c>
       <c r="C90">
-        <v>0.0007995353883215832</v>
+        <v>0.006078689041967155</v>
       </c>
       <c r="D90">
-        <v>5.249110074922114e-06</v>
+        <v>5.810391422817444e-05</v>
       </c>
       <c r="E90">
-        <v>0.0003905807997092933</v>
+        <v>0.004019657560082311</v>
       </c>
       <c r="F90">
-        <v>0.0001604377971656712</v>
+        <v>0.001754251494885556</v>
       </c>
       <c r="G90">
-        <v>4.908598477224948e-07</v>
+        <v>2.824643462843366e-06</v>
       </c>
       <c r="H90">
-        <v>0.001857638978425741</v>
+        <v>0.01963403493900283</v>
       </c>
     </row>
     <row r="91" spans="1:8">
@@ -2740,25 +2740,25 @@
         <v>89</v>
       </c>
       <c r="B91">
-        <v>0.0004345455677265378</v>
+        <v>0.005888075280754823</v>
       </c>
       <c r="C91">
-        <v>0.0004334872507647719</v>
+        <v>0.003404782736284978</v>
       </c>
       <c r="D91">
-        <v>5.28201570046697e-06</v>
+        <v>4.69630095770945e-05</v>
       </c>
       <c r="E91">
-        <v>0.0004573894860435541</v>
+        <v>0.003233364224873692</v>
       </c>
       <c r="F91">
-        <v>0.0001383238720841102</v>
+        <v>0.001230645279889738</v>
       </c>
       <c r="G91">
-        <v>4.690855120968629e-07</v>
+        <v>2.221970072381153e-06</v>
       </c>
       <c r="H91">
-        <v>0.001668018008211174</v>
+        <v>0.01370801806518659</v>
       </c>
     </row>
     <row r="92" spans="1:8">
@@ -2766,25 +2766,25 @@
         <v>90</v>
       </c>
       <c r="B92">
-        <v>0.0004929580478397747</v>
+        <v>0.006603544810649594</v>
       </c>
       <c r="C92">
-        <v>0.0007713305412035416</v>
+        <v>0.004477465663775111</v>
       </c>
       <c r="D92">
-        <v>5.174523594822014e-06</v>
+        <v>6.850813305715107e-05</v>
       </c>
       <c r="E92">
-        <v>0.0003741819441832634</v>
+        <v>0.003212956320747056</v>
       </c>
       <c r="F92">
-        <v>0.0001420200736214285</v>
+        <v>0.00170502364930642</v>
       </c>
       <c r="G92">
-        <v>5.585135243552686e-07</v>
+        <v>2.631459353831062e-06</v>
       </c>
       <c r="H92">
-        <v>0.001644862366563288</v>
+        <v>0.01797746975714288</v>
       </c>
     </row>
     <row r="93" spans="1:8">
@@ -2792,25 +2792,25 @@
         <v>91</v>
       </c>
       <c r="B93">
-        <v>0.0004118597963258512</v>
+        <v>0.009333610871674183</v>
       </c>
       <c r="C93">
-        <v>0.0005945356990335046</v>
+        <v>0.005154936817347585</v>
       </c>
       <c r="D93">
-        <v>4.696550766491097e-06</v>
+        <v>7.931399583846704e-05</v>
       </c>
       <c r="E93">
-        <v>0.0003601944841128885</v>
+        <v>0.004258558746557186</v>
       </c>
       <c r="F93">
-        <v>0.0001287699760389162</v>
+        <v>0.001753360111209153</v>
       </c>
       <c r="G93">
-        <v>4.877594073866137e-07</v>
+        <v>3.097489978765693e-06</v>
       </c>
       <c r="H93">
-        <v>0.001374958715939216</v>
+        <v>0.01940573293288305</v>
       </c>
     </row>
     <row r="94" spans="1:8">
@@ -2818,25 +2818,25 @@
         <v>92</v>
       </c>
       <c r="B94">
-        <v>0.0004675755429770062</v>
+        <v>0.007533292346006341</v>
       </c>
       <c r="C94">
-        <v>0.0004865244739109817</v>
+        <v>0.005215912778807052</v>
       </c>
       <c r="D94">
-        <v>5.061565297504669e-06</v>
+        <v>6.991732014044887e-05</v>
       </c>
       <c r="E94">
-        <v>0.0003927668351104649</v>
+        <v>0.003816954922955789</v>
       </c>
       <c r="F94">
-        <v>0.0001768990494271715</v>
+        <v>0.001803378553911265</v>
       </c>
       <c r="G94">
-        <v>5.895528349805186e-07</v>
+        <v>2.84051870726945e-06</v>
       </c>
       <c r="H94">
-        <v>0.001948712167883383</v>
+        <v>0.01937378543694181</v>
       </c>
     </row>
     <row r="95" spans="1:8">
@@ -2844,25 +2844,25 @@
         <v>93</v>
       </c>
       <c r="B95">
-        <v>0.000440314067129247</v>
+        <v>0.006253105052240072</v>
       </c>
       <c r="C95">
-        <v>0.0006584422262789125</v>
+        <v>0.004445042218629732</v>
       </c>
       <c r="D95">
-        <v>5.703163792579637e-06</v>
+        <v>6.413300993512166e-05</v>
       </c>
       <c r="E95">
-        <v>0.0003695999231442171</v>
+        <v>0.003612276951129601</v>
       </c>
       <c r="F95">
-        <v>0.0001522170818034745</v>
+        <v>0.001510689308024127</v>
       </c>
       <c r="G95">
-        <v>5.879237727856384e-07</v>
+        <v>2.708914754958687e-06</v>
       </c>
       <c r="H95">
-        <v>0.001476543762348116</v>
+        <v>0.01652138389120042</v>
       </c>
     </row>
     <row r="96" spans="1:8">
@@ -2870,25 +2870,25 @@
         <v>94</v>
       </c>
       <c r="B96">
-        <v>0.000386676963460654</v>
+        <v>0.005577207513716973</v>
       </c>
       <c r="C96">
-        <v>0.000469143641318496</v>
+        <v>0.005172513333887521</v>
       </c>
       <c r="D96">
-        <v>4.023773793527933e-06</v>
+        <v>4.373737623599981e-05</v>
       </c>
       <c r="E96">
-        <v>0.0003495437770786193</v>
+        <v>0.002796053942495812</v>
       </c>
       <c r="F96">
-        <v>0.0001797205277589518</v>
+        <v>0.001391607313187378</v>
       </c>
       <c r="G96">
-        <v>5.230978618231623e-07</v>
+        <v>2.209289036514548e-06</v>
       </c>
       <c r="H96">
-        <v>0.001934039541318679</v>
+        <v>0.01525059045323078</v>
       </c>
     </row>
     <row r="97" spans="1:8">
@@ -2896,25 +2896,25 @@
         <v>95</v>
       </c>
       <c r="B97">
-        <v>0.0004166122675381443</v>
+        <v>0.005212467648624733</v>
       </c>
       <c r="C97">
-        <v>0.0004715119002409589</v>
+        <v>0.003938845248751581</v>
       </c>
       <c r="D97">
-        <v>3.695638729725624e-06</v>
+        <v>5.344033775815091e-05</v>
       </c>
       <c r="E97">
-        <v>0.0003351395604991639</v>
+        <v>0.003055794023954823</v>
       </c>
       <c r="F97">
-        <v>0.0001079401254051314</v>
+        <v>0.001374567686510234</v>
       </c>
       <c r="G97">
-        <v>4.715150392892662e-07</v>
+        <v>2.295993357823754e-06</v>
       </c>
       <c r="H97">
-        <v>0.001326967974132903</v>
+        <v>0.01496075461082949</v>
       </c>
     </row>
     <row r="98" spans="1:8">
@@ -2922,25 +2922,25 @@
         <v>96</v>
       </c>
       <c r="B98">
-        <v>0.0004351335603999012</v>
+        <v>0.007003190433808038</v>
       </c>
       <c r="C98">
-        <v>0.0005220315997708594</v>
+        <v>0.005042784649638104</v>
       </c>
       <c r="D98">
-        <v>4.868520962658719e-06</v>
+        <v>6.729615752519393e-05</v>
       </c>
       <c r="E98">
-        <v>0.000366428670246016</v>
+        <v>0.003851887934819585</v>
       </c>
       <c r="F98">
-        <v>0.0001593775927614425</v>
+        <v>0.001423481084774287</v>
       </c>
       <c r="G98">
-        <v>5.736090505912671e-07</v>
+        <v>2.288753800498073e-06</v>
       </c>
       <c r="H98">
-        <v>0.001729523286409887</v>
+        <v>0.01691787688519742</v>
       </c>
     </row>
     <row r="99" spans="1:8">
@@ -2948,25 +2948,25 @@
         <v>97</v>
       </c>
       <c r="B99">
-        <v>0.0004217064752206056</v>
+        <v>0.008173360856752149</v>
       </c>
       <c r="C99">
-        <v>0.0005359834344439046</v>
+        <v>0.005856430936679892</v>
       </c>
       <c r="D99">
-        <v>6.775404996599975e-06</v>
+        <v>6.999626075981356e-05</v>
       </c>
       <c r="E99">
-        <v>0.0003099074824673245</v>
+        <v>0.003445044131029279</v>
       </c>
       <c r="F99">
-        <v>0.0001668897824569369</v>
+        <v>0.001884479735342359</v>
       </c>
       <c r="G99">
-        <v>6.04407267526902e-07</v>
+        <v>3.286916242494011e-06</v>
       </c>
       <c r="H99">
-        <v>0.001676004606994927</v>
+        <v>0.01983338533907313</v>
       </c>
     </row>
     <row r="100" spans="1:8">
@@ -2974,25 +2974,25 @@
         <v>98</v>
       </c>
       <c r="B100">
-        <v>0.0003767658495333445</v>
+        <v>0.007748651416370021</v>
       </c>
       <c r="C100">
-        <v>0.0005270470886446926</v>
+        <v>0.005961002364241266</v>
       </c>
       <c r="D100">
-        <v>5.904024670129608e-06</v>
+        <v>6.801036225182161e-05</v>
       </c>
       <c r="E100">
-        <v>0.0003680920446047945</v>
+        <v>0.003362614322394012</v>
       </c>
       <c r="F100">
-        <v>0.0001391787817258929</v>
+        <v>0.001526432654442597</v>
       </c>
       <c r="G100">
-        <v>4.737566958774273e-07</v>
+        <v>2.67242840823422e-06</v>
       </c>
       <c r="H100">
-        <v>0.001578937596307153</v>
+        <v>0.0163907965168126</v>
       </c>
     </row>
     <row r="101" spans="1:8">
@@ -3000,25 +3000,25 @@
         <v>99</v>
       </c>
       <c r="B101">
-        <v>0.0004826695553722992</v>
+        <v>0.006500749358811004</v>
       </c>
       <c r="C101">
-        <v>0.0006479409105551012</v>
+        <v>0.005321041792709879</v>
       </c>
       <c r="D101">
-        <v>4.746491436899585e-06</v>
+        <v>5.317978196667925e-05</v>
       </c>
       <c r="E101">
-        <v>0.0002899798630572495</v>
+        <v>0.003424051853819803</v>
       </c>
       <c r="F101">
-        <v>0.0001513580369090166</v>
+        <v>0.00154402925827547</v>
       </c>
       <c r="G101">
-        <v>5.243807136705544e-07</v>
+        <v>2.491351603412871e-06</v>
       </c>
       <c r="H101">
-        <v>0.001624772263935655</v>
+        <v>0.01691583107733601</v>
       </c>
     </row>
     <row r="102" spans="1:8">
@@ -3026,25 +3026,25 @@
         <v>100</v>
       </c>
       <c r="B102">
-        <v>0.0004804040821244214</v>
+        <v>0.006023718594156227</v>
       </c>
       <c r="C102">
-        <v>0.0004586566364958578</v>
+        <v>0.003958008726840791</v>
       </c>
       <c r="D102">
-        <v>5.777351661290752e-06</v>
+        <v>4.85136563228428e-05</v>
       </c>
       <c r="E102">
-        <v>0.0002865519904422295</v>
+        <v>0.00342682652409963</v>
       </c>
       <c r="F102">
-        <v>0.0001871318538702912</v>
+        <v>0.001457490868247974</v>
       </c>
       <c r="G102">
-        <v>6.511184814180023e-07</v>
+        <v>2.188450536057046e-06</v>
       </c>
       <c r="H102">
-        <v>0.001999805985456586</v>
+        <v>0.01644880989496573</v>
       </c>
     </row>
     <row r="103" spans="1:8">
@@ -3052,25 +3052,25 @@
         <v>101</v>
       </c>
       <c r="B103">
-        <v>0.0006197378307147379</v>
+        <v>0.007413540153959217</v>
       </c>
       <c r="C103">
-        <v>0.0006270670544826435</v>
+        <v>0.004188369407590091</v>
       </c>
       <c r="D103">
-        <v>5.430282548852753e-06</v>
+        <v>6.036930177154967e-05</v>
       </c>
       <c r="E103">
-        <v>0.0003793274913193086</v>
+        <v>0.003753116767027855</v>
       </c>
       <c r="F103">
-        <v>0.000156718230291355</v>
+        <v>0.001609192060275172</v>
       </c>
       <c r="G103">
-        <v>6.064565857827904e-07</v>
+        <v>2.301773495916264e-06</v>
       </c>
       <c r="H103">
-        <v>0.001884100599977909</v>
+        <v>0.01829319072296688</v>
       </c>
     </row>
     <row r="104" spans="1:8">
@@ -3078,25 +3078,25 @@
         <v>102</v>
       </c>
       <c r="B104">
-        <v>0.0005156695221050603</v>
+        <v>0.00653875488245362</v>
       </c>
       <c r="C104">
-        <v>0.0004721769780612648</v>
+        <v>0.007877620066584575</v>
       </c>
       <c r="D104">
-        <v>5.974716172122309e-06</v>
+        <v>5.711620770003997e-05</v>
       </c>
       <c r="E104">
-        <v>0.0002988252310282149</v>
+        <v>0.003969850597688108</v>
       </c>
       <c r="F104">
-        <v>0.0001377396827506941</v>
+        <v>0.002120870881782162</v>
       </c>
       <c r="G104">
-        <v>6.795110243746612e-07</v>
+        <v>3.258803755870548e-06</v>
       </c>
       <c r="H104">
-        <v>0.001527241646081304</v>
+        <v>0.02204568965449077</v>
       </c>
     </row>
     <row r="105" spans="1:8">
@@ -3104,25 +3104,25 @@
         <v>103</v>
       </c>
       <c r="B105">
-        <v>0.0004377452345337518</v>
+        <v>0.007057263275671928</v>
       </c>
       <c r="C105">
-        <v>0.000395403573140643</v>
+        <v>0.005281859489740868</v>
       </c>
       <c r="D105">
-        <v>5.081589657954254e-06</v>
+        <v>7.653025523103322e-05</v>
       </c>
       <c r="E105">
-        <v>0.0005191910470126867</v>
+        <v>0.002915064135493443</v>
       </c>
       <c r="F105">
-        <v>0.0001741471162304067</v>
+        <v>0.001886098443629622</v>
       </c>
       <c r="G105">
-        <v>7.753584957651447e-07</v>
+        <v>3.391846188412408e-06</v>
       </c>
       <c r="H105">
-        <v>0.002042646660085931</v>
+        <v>0.02055279885699578</v>
       </c>
     </row>
     <row r="106" spans="1:8">
@@ -3130,25 +3130,25 @@
         <v>104</v>
       </c>
       <c r="B106">
-        <v>0.0004384495037088918</v>
+        <v>0.006542381134477793</v>
       </c>
       <c r="C106">
-        <v>0.0005791313811114844</v>
+        <v>0.005765787465592326</v>
       </c>
       <c r="D106">
-        <v>6.127645260557166e-06</v>
+        <v>6.402139197893448e-05</v>
       </c>
       <c r="E106">
-        <v>0.0003348157810487785</v>
+        <v>0.003772757469515006</v>
       </c>
       <c r="F106">
-        <v>0.0001255986105939746</v>
+        <v>0.00186681958094211</v>
       </c>
       <c r="G106">
-        <v>5.547667910529043e-07</v>
+        <v>2.978431208411949e-06</v>
       </c>
       <c r="H106">
-        <v>0.001479805219675183</v>
+        <v>0.01956635910710216</v>
       </c>
     </row>
     <row r="107" spans="1:8">
@@ -3156,25 +3156,25 @@
         <v>105</v>
       </c>
       <c r="B107">
-        <v>0.0003594479553012573</v>
+        <v>0.007261855109658388</v>
       </c>
       <c r="C107">
-        <v>0.0005103340082458043</v>
+        <v>0.006290986235449647</v>
       </c>
       <c r="D107">
-        <v>3.931022307701535e-06</v>
+        <v>5.840557486228856e-05</v>
       </c>
       <c r="E107">
-        <v>0.000340738545232224</v>
+        <v>0.004255970513333116</v>
       </c>
       <c r="F107">
-        <v>0.000139254091043171</v>
+        <v>0.001835736404241746</v>
       </c>
       <c r="G107">
-        <v>4.574871423634372e-07</v>
+        <v>2.527893706300993e-06</v>
       </c>
       <c r="H107">
-        <v>0.001523383458642044</v>
+        <v>0.02140232783696948</v>
       </c>
     </row>
     <row r="108" spans="1:8">
@@ -3182,25 +3182,25 @@
         <v>106</v>
       </c>
       <c r="B108">
-        <v>0.000471903471315001</v>
+        <v>0.007671091009056306</v>
       </c>
       <c r="C108">
-        <v>0.0004249635171283246</v>
+        <v>0.004908070645454056</v>
       </c>
       <c r="D108">
-        <v>4.958370261318657e-06</v>
+        <v>7.89337072424836e-05</v>
       </c>
       <c r="E108">
-        <v>0.0003492367272356255</v>
+        <v>0.003655542463633142</v>
       </c>
       <c r="F108">
-        <v>0.0001585948036888643</v>
+        <v>0.001496543978796923</v>
       </c>
       <c r="G108">
-        <v>5.044226673960665e-07</v>
+        <v>2.562391242284654e-06</v>
       </c>
       <c r="H108">
-        <v>0.001771591941048082</v>
+        <v>0.01792207435184808</v>
       </c>
     </row>
     <row r="109" spans="1:8">
@@ -3208,25 +3208,25 @@
         <v>107</v>
       </c>
       <c r="B109">
-        <v>0.0004398276991875091</v>
+        <v>0.008100165910893201</v>
       </c>
       <c r="C109">
-        <v>0.0004467441996336525</v>
+        <v>0.005586215487217753</v>
       </c>
       <c r="D109">
-        <v>4.331595657749936e-06</v>
+        <v>7.930406988065118e-05</v>
       </c>
       <c r="E109">
-        <v>0.0003563175328541053</v>
+        <v>0.004412557205870702</v>
       </c>
       <c r="F109">
-        <v>0.0001683188469173098</v>
+        <v>0.001674035032240301</v>
       </c>
       <c r="G109">
-        <v>4.485338614298392e-07</v>
+        <v>2.604352802914799e-06</v>
       </c>
       <c r="H109">
-        <v>0.00185568166348161</v>
+        <v>0.0179781619161321</v>
       </c>
     </row>
     <row r="110" spans="1:8">
@@ -3234,25 +3234,25 @@
         <v>108</v>
       </c>
       <c r="B110">
-        <v>0.0004834752727425904</v>
+        <v>0.005535210369825022</v>
       </c>
       <c r="C110">
-        <v>0.00043104375801858</v>
+        <v>0.005617808904314008</v>
       </c>
       <c r="D110">
-        <v>5.792637920792623e-06</v>
+        <v>5.445324911835347e-05</v>
       </c>
       <c r="E110">
-        <v>0.000316477054154773</v>
+        <v>0.003446276953098017</v>
       </c>
       <c r="F110">
-        <v>0.0001600594373043779</v>
+        <v>0.001587160348872659</v>
       </c>
       <c r="G110">
-        <v>5.810225748242869e-07</v>
+        <v>2.755300899454535e-06</v>
       </c>
       <c r="H110">
-        <v>0.001639201321548382</v>
+        <v>0.0166939067471166</v>
       </c>
     </row>
     <row r="111" spans="1:8">
@@ -3260,25 +3260,25 @@
         <v>109</v>
       </c>
       <c r="B111">
-        <v>0.0004412115020808121</v>
+        <v>0.009675714562069081</v>
       </c>
       <c r="C111">
-        <v>0.0008029432945366357</v>
+        <v>0.005738034118174896</v>
       </c>
       <c r="D111">
-        <v>4.623529339008188e-06</v>
+        <v>6.249142979514686e-05</v>
       </c>
       <c r="E111">
-        <v>0.0003118020390916544</v>
+        <v>0.005187386673168887</v>
       </c>
       <c r="F111">
-        <v>0.0001502284905257064</v>
+        <v>0.002220156168040783</v>
       </c>
       <c r="G111">
-        <v>5.044848688125391e-07</v>
+        <v>2.912912638264307e-06</v>
       </c>
       <c r="H111">
-        <v>0.001660870454360789</v>
+        <v>0.02617972878204501</v>
       </c>
     </row>
     <row r="112" spans="1:8">
@@ -3286,25 +3286,25 @@
         <v>110</v>
       </c>
       <c r="B112">
-        <v>0.0005237356373052579</v>
+        <v>0.006232474408747</v>
       </c>
       <c r="C112">
-        <v>0.0004381303428982252</v>
+        <v>0.006006451614370483</v>
       </c>
       <c r="D112">
-        <v>5.359780846728059e-06</v>
+        <v>6.756945770068856e-05</v>
       </c>
       <c r="E112">
-        <v>0.0003543159357274458</v>
+        <v>0.003344084988276996</v>
       </c>
       <c r="F112">
-        <v>0.0001640156980968154</v>
+        <v>0.001842136932961328</v>
       </c>
       <c r="G112">
-        <v>5.855711580331342e-07</v>
+        <v>3.092085254165382e-06</v>
       </c>
       <c r="H112">
-        <v>0.001859247796508362</v>
+        <v>0.01955818988459675</v>
       </c>
     </row>
     <row r="113" spans="1:8">
@@ -3312,25 +3312,25 @@
         <v>111</v>
       </c>
       <c r="B113">
-        <v>0.0003919102063853325</v>
+        <v>0.007163966743166919</v>
       </c>
       <c r="C113">
-        <v>0.0004543207797214349</v>
+        <v>0.005359393897630692</v>
       </c>
       <c r="D113">
-        <v>5.496762138502021e-06</v>
+        <v>5.936111915646827e-05</v>
       </c>
       <c r="E113">
-        <v>0.0003098445032279205</v>
+        <v>0.004067113462535736</v>
       </c>
       <c r="F113">
-        <v>0.0001542117281922946</v>
+        <v>0.001692565945101599</v>
       </c>
       <c r="G113">
-        <v>5.001325824305549e-07</v>
+        <v>2.752211346046799e-06</v>
       </c>
       <c r="H113">
-        <v>0.001607051201967568</v>
+        <v>0.01924816194099402</v>
       </c>
     </row>
     <row r="114" spans="1:8">
@@ -3338,25 +3338,25 @@
         <v>112</v>
       </c>
       <c r="B114">
-        <v>0.0005662992406180797</v>
+        <v>0.007414579996830337</v>
       </c>
       <c r="C114">
-        <v>0.0003704328356758418</v>
+        <v>0.006073884525836877</v>
       </c>
       <c r="D114">
-        <v>4.963686863829214e-06</v>
+        <v>6.848113375812699e-05</v>
       </c>
       <c r="E114">
-        <v>0.0003149189945388548</v>
+        <v>0.00360446173295188</v>
       </c>
       <c r="F114">
-        <v>0.0001793092128762105</v>
+        <v>0.00186922114689677</v>
       </c>
       <c r="G114">
-        <v>5.666380882865299e-07</v>
+        <v>2.880920650609285e-06</v>
       </c>
       <c r="H114">
-        <v>0.002099215297192801</v>
+        <v>0.02028874473334652</v>
       </c>
     </row>
     <row r="115" spans="1:8">
@@ -3364,25 +3364,25 @@
         <v>113</v>
       </c>
       <c r="B115">
-        <v>0.0004027984129341665</v>
+        <v>0.006300240438421538</v>
       </c>
       <c r="C115">
-        <v>0.0004207650073944248</v>
+        <v>0.005376971170822511</v>
       </c>
       <c r="D115">
-        <v>4.561555430719344e-06</v>
+        <v>6.578947373518573e-05</v>
       </c>
       <c r="E115">
-        <v>0.0003257406448395911</v>
+        <v>0.003127806369385185</v>
       </c>
       <c r="F115">
-        <v>0.0001334322574695126</v>
+        <v>0.002014776890290295</v>
       </c>
       <c r="G115">
-        <v>5.33685967633783e-07</v>
+        <v>3.276645075942772e-06</v>
       </c>
       <c r="H115">
-        <v>0.001441104157321542</v>
+        <v>0.02057512564340543</v>
       </c>
     </row>
     <row r="116" spans="1:8">
@@ -3390,25 +3390,25 @@
         <v>114</v>
       </c>
       <c r="B116">
-        <v>0.0004041631467850352</v>
+        <v>0.007025610392662188</v>
       </c>
       <c r="C116">
-        <v>0.0004838635633816738</v>
+        <v>0.005299126744491399</v>
       </c>
       <c r="D116">
-        <v>5.1721172318804e-06</v>
+        <v>6.538280446189222e-05</v>
       </c>
       <c r="E116">
-        <v>0.0003768651199689624</v>
+        <v>0.003305042477581778</v>
       </c>
       <c r="F116">
-        <v>0.0001675295012649829</v>
+        <v>0.001557722940078761</v>
       </c>
       <c r="G116">
-        <v>6.392731613004534e-07</v>
+        <v>2.551986893079686e-06</v>
       </c>
       <c r="H116">
-        <v>0.001858576394114057</v>
+        <v>0.01709020800266009</v>
       </c>
     </row>
     <row r="117" spans="1:8">
@@ -3416,25 +3416,25 @@
         <v>115</v>
       </c>
       <c r="B117">
-        <v>0.0004724687467862964</v>
+        <v>0.006999884284439923</v>
       </c>
       <c r="C117">
-        <v>0.0005047188253703925</v>
+        <v>0.006316162748758023</v>
       </c>
       <c r="D117">
-        <v>5.311313122483714e-06</v>
+        <v>7.288072092877145e-05</v>
       </c>
       <c r="E117">
-        <v>0.000422644374991337</v>
+        <v>0.003235527840527374</v>
       </c>
       <c r="F117">
-        <v>0.0001662582207671915</v>
+        <v>0.001639674828696877</v>
       </c>
       <c r="G117">
-        <v>7.125726222207903e-07</v>
+        <v>2.48206174196728e-06</v>
       </c>
       <c r="H117">
-        <v>0.001725307172205063</v>
+        <v>0.0184896460061301</v>
       </c>
     </row>
     <row r="118" spans="1:8">
@@ -3442,25 +3442,25 @@
         <v>116</v>
       </c>
       <c r="B118">
-        <v>0.0004946169500123771</v>
+        <v>0.007079851711031853</v>
       </c>
       <c r="C118">
-        <v>0.0004615728039319853</v>
+        <v>0.005766218928577028</v>
       </c>
       <c r="D118">
-        <v>6.40973003880187e-06</v>
+        <v>5.770311526156329e-05</v>
       </c>
       <c r="E118">
-        <v>0.0004101732958917096</v>
+        <v>0.003896171787947138</v>
       </c>
       <c r="F118">
-        <v>0.0001511111971457525</v>
+        <v>0.001904733847930455</v>
       </c>
       <c r="G118">
-        <v>5.780701303457615e-07</v>
+        <v>3.548644914141335e-06</v>
       </c>
       <c r="H118">
-        <v>0.001823625437102091</v>
+        <v>0.02193100260329634</v>
       </c>
     </row>
     <row r="119" spans="1:8">
@@ -3468,25 +3468,25 @@
         <v>117</v>
       </c>
       <c r="B119">
-        <v>0.0005228765240872447</v>
+        <v>0.007268916165608102</v>
       </c>
       <c r="C119">
-        <v>0.0004126307812724622</v>
+        <v>0.005295728330664805</v>
       </c>
       <c r="D119">
-        <v>4.060406576502495e-06</v>
+        <v>5.544985255593302e-05</v>
       </c>
       <c r="E119">
-        <v>0.0002942866463379774</v>
+        <v>0.003859021566525936</v>
       </c>
       <c r="F119">
-        <v>0.000173950691311731</v>
+        <v>0.001687196806706975</v>
       </c>
       <c r="G119">
-        <v>6.588671894663155e-07</v>
+        <v>2.342713697437585e-06</v>
       </c>
       <c r="H119">
-        <v>0.001958186963961831</v>
+        <v>0.02089237401495473</v>
       </c>
     </row>
     <row r="120" spans="1:8">
@@ -3494,25 +3494,25 @@
         <v>118</v>
       </c>
       <c r="B120">
-        <v>0.0004771791923392143</v>
+        <v>0.009190871408286326</v>
       </c>
       <c r="C120">
-        <v>0.0005397441207745405</v>
+        <v>0.004999743594926198</v>
       </c>
       <c r="D120">
-        <v>5.045587958368124e-06</v>
+        <v>8.040375989600895e-05</v>
       </c>
       <c r="E120">
-        <v>0.0002880608405568137</v>
+        <v>0.003524146776689567</v>
       </c>
       <c r="F120">
-        <v>0.0001715611154615473</v>
+        <v>0.002068791532031516</v>
       </c>
       <c r="G120">
-        <v>6.042417009798896e-07</v>
+        <v>3.522821129833696e-06</v>
       </c>
       <c r="H120">
-        <v>0.001978477315623375</v>
+        <v>0.02145898197150925</v>
       </c>
     </row>
     <row r="121" spans="1:8">
@@ -3520,25 +3520,25 @@
         <v>119</v>
       </c>
       <c r="B121">
-        <v>0.000407148785869516</v>
+        <v>0.007015840569822748</v>
       </c>
       <c r="C121">
-        <v>0.0005464621965785036</v>
+        <v>0.004543563170572393</v>
       </c>
       <c r="D121">
-        <v>4.997061864866867e-06</v>
+        <v>7.063505526924208e-05</v>
       </c>
       <c r="E121">
-        <v>0.0005081488010560319</v>
+        <v>0.003027310034719892</v>
       </c>
       <c r="F121">
-        <v>0.0001353871044570852</v>
+        <v>0.001464969887193891</v>
       </c>
       <c r="G121">
-        <v>4.6873986724311e-07</v>
+        <v>2.614348336960954e-06</v>
       </c>
       <c r="H121">
-        <v>0.001314000653525833</v>
+        <v>0.01704230372572781</v>
       </c>
     </row>
   </sheetData>

</xml_diff>